<commit_message>
merge scenarios from master
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="91">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -223,6 +223,75 @@
   </si>
   <si>
     <t>increase</t>
+  </si>
+  <si>
+    <t>fixed - 1 forecast</t>
+  </si>
+  <si>
+    <t>internal - 1 forecast</t>
+  </si>
+  <si>
+    <t>No age comp data for any fleet</t>
+  </si>
+  <si>
+    <t>Age comp data for the fishery</t>
+  </si>
+  <si>
+    <t>Age comp data for the fishery and every other year of total survey years</t>
+  </si>
+  <si>
+    <t>Age comp data for the fishery and for every year of the total survey years</t>
+  </si>
+  <si>
+    <t>No conditional age at length data</t>
+  </si>
+  <si>
+    <t>Fishery conditional age at length data</t>
+  </si>
+  <si>
+    <t>No mean length at age data</t>
+  </si>
+  <si>
+    <t>Fishery mean length at age data</t>
+  </si>
+  <si>
+    <t>Survey conditional age at length data</t>
+  </si>
+  <si>
+    <t>Survey mean length at age data</t>
+  </si>
+  <si>
+    <t>all growth parameters fixed at their true values</t>
+  </si>
+  <si>
+    <t>all growth parameters are estimated internally</t>
+  </si>
+  <si>
+    <t>all growth parameters are estimated using Christine's external function</t>
+  </si>
+  <si>
+    <t>all growth parameters are fixed at their true values and one year of forecasting is done</t>
+  </si>
+  <si>
+    <t>all growth parameters are estimated internally and one year of forecasting is done</t>
+  </si>
+  <si>
+    <t>Constant fishing at  a percentage of FMSY</t>
+  </si>
+  <si>
+    <t>Two way trip</t>
+  </si>
+  <si>
+    <t>A one way trip fishing scenario</t>
+  </si>
+  <si>
+    <t>Fishery length composition data and every other year of composition data from the survey years</t>
+  </si>
+  <si>
+    <t>Fishery length composition data and every year of composition data from the survey years</t>
+  </si>
+  <si>
+    <t>Fishery length composition data</t>
   </si>
 </sst>
 </file>
@@ -574,7 +643,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N169"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
@@ -9211,10 +9280,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9250,6 +9319,9 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -9259,11 +9331,14 @@
         <v>10</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C20" si="0">CONCATENATE(A3,B3)</f>
+        <f t="shared" ref="C3:C22" si="0">CONCATENATE(A3,B3)</f>
         <v>A10</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -9280,6 +9355,9 @@
       <c r="D4" t="s">
         <v>46</v>
       </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -9295,6 +9373,9 @@
       <c r="D5" t="s">
         <v>47</v>
       </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -9310,6 +9391,9 @@
       <c r="D6" t="s">
         <v>16</v>
       </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -9325,6 +9409,9 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -9340,6 +9427,9 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -9355,6 +9445,9 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -9370,6 +9463,9 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -9385,6 +9481,9 @@
       <c r="D11" t="s">
         <v>1</v>
       </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -9400,6 +9499,9 @@
       <c r="D12" t="s">
         <v>52</v>
       </c>
+      <c r="E12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -9415,6 +9517,9 @@
       <c r="D13" t="s">
         <v>53</v>
       </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -9430,95 +9535,152 @@
       <c r="D14" t="s">
         <v>54</v>
       </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>990</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>F0</v>
+        <v>E990</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>991</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>F1</v>
+        <v>E991</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F0</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>L10</v>
+        <v>F1</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>L30</v>
+        <v>F2</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
       <c r="B20">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
+        <v>L10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>L30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
         <v>L31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix descriptions for 30 and 31
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine Stawitz\Documents\GitHub\estgrowth\lib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$39</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="63">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -150,12 +145,6 @@
   </si>
   <si>
     <t>descriptionlong</t>
-  </si>
-  <si>
-    <t>fish &amp; .5surv age</t>
-  </si>
-  <si>
-    <t>fish &amp; surv age</t>
   </si>
   <si>
     <t>C</t>
@@ -326,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -575,21 +564,21 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -606,7 +595,7 @@
         <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
@@ -630,10 +619,10 @@
         <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -650,10 +639,10 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(A2,"-",B2,"-",C2,"-",D2,"-",E2,"-",F2,"-",G2,"-")</f>
@@ -684,7 +673,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -701,10 +690,10 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H28" si="0">CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
@@ -724,7 +713,7 @@
       </c>
       <c r="L3" t="str">
         <f>LOOKUP(D3,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M3" t="str">
         <f>LOOKUP(E3,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -735,7 +724,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -752,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -786,7 +775,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -803,10 +792,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -826,7 +815,7 @@
       </c>
       <c r="L5" t="str">
         <f>LOOKUP(D5,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M5" t="str">
         <f>LOOKUP(E5,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -837,7 +826,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -854,10 +843,10 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -888,7 +877,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -905,10 +894,10 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -928,7 +917,7 @@
       </c>
       <c r="L7" t="str">
         <f>LOOKUP(D7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M7" t="str">
         <f>LOOKUP(E7,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -939,7 +928,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -956,10 +945,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -990,7 +979,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1007,10 +996,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1030,7 +1019,7 @@
       </c>
       <c r="L9" t="str">
         <f>LOOKUP(D9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M9" t="str">
         <f>LOOKUP(E9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1041,7 +1030,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1058,10 +1047,10 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1092,7 +1081,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1109,10 +1098,10 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1132,7 +1121,7 @@
       </c>
       <c r="L11" t="str">
         <f>LOOKUP(D11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M11" t="str">
         <f>LOOKUP(E11,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1143,7 +1132,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1160,10 +1149,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1194,7 +1183,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1211,10 +1200,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1234,7 +1223,7 @@
       </c>
       <c r="L13" t="str">
         <f>LOOKUP(D13,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M13" t="str">
         <f>LOOKUP(E13,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1245,7 +1234,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1262,10 +1251,10 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1296,7 +1285,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1313,10 +1302,10 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1336,7 +1325,7 @@
       </c>
       <c r="L15" t="str">
         <f>LOOKUP(D15,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M15" t="str">
         <f>LOOKUP(E15,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1347,7 +1336,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1364,10 +1353,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1398,7 +1387,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1415,10 +1404,10 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -1438,7 +1427,7 @@
       </c>
       <c r="L17" t="str">
         <f>LOOKUP(D17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M17" t="str">
         <f>LOOKUP(E17,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1449,7 +1438,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1466,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -1500,7 +1489,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1517,10 +1506,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1551,7 +1540,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1568,10 +1557,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -1591,7 +1580,7 @@
       </c>
       <c r="L20" t="str">
         <f>LOOKUP(D20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M20" t="str">
         <f>LOOKUP(E20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1602,7 +1591,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1619,10 +1608,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1642,7 +1631,7 @@
       </c>
       <c r="L21" t="str">
         <f>LOOKUP(D21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M21" t="str">
         <f>LOOKUP(E21,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1653,7 +1642,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1670,10 +1659,10 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1681,7 +1670,7 @@
       </c>
       <c r="I22" t="str">
         <f>LOOKUP(A22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J22" t="str">
         <f>LOOKUP(B22,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1704,7 +1693,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1721,10 +1710,10 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1732,7 +1721,7 @@
       </c>
       <c r="I23" t="str">
         <f>LOOKUP(A23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J23" t="str">
         <f>LOOKUP(B23,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1744,7 +1733,7 @@
       </c>
       <c r="L23" t="str">
         <f>LOOKUP(D23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M23" t="str">
         <f>LOOKUP(E23,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1755,7 +1744,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1772,10 +1761,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1783,7 +1772,7 @@
       </c>
       <c r="I24" t="str">
         <f>LOOKUP(A24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J24" t="str">
         <f>LOOKUP(B24,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1806,7 +1795,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1823,10 +1812,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -1834,7 +1823,7 @@
       </c>
       <c r="I25" t="str">
         <f>LOOKUP(A25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J25" t="str">
         <f>LOOKUP(B25,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1846,7 +1835,7 @@
       </c>
       <c r="L25" t="str">
         <f>LOOKUP(D25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M25" t="str">
         <f>LOOKUP(E25,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1857,7 +1846,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1874,10 +1863,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -1885,7 +1874,7 @@
       </c>
       <c r="I26" t="str">
         <f>LOOKUP(A26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J26" t="str">
         <f>LOOKUP(B26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1908,7 +1897,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1925,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -1936,7 +1925,7 @@
       </c>
       <c r="I27" t="str">
         <f>LOOKUP(A27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J27" t="str">
         <f>LOOKUP(B27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1959,7 +1948,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1976,10 +1965,10 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -1987,7 +1976,7 @@
       </c>
       <c r="I28" t="str">
         <f>LOOKUP(A28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J28" t="str">
         <f>LOOKUP(B28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1999,7 +1988,7 @@
       </c>
       <c r="L28" t="str">
         <f>LOOKUP(D28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M28" t="str">
         <f>LOOKUP(E28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2010,7 +1999,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -2027,10 +2016,10 @@
         <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" ref="H29:H39" si="1">CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
@@ -2038,7 +2027,7 @@
       </c>
       <c r="I29" t="str">
         <f>LOOKUP(A29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J29" t="str">
         <f>LOOKUP(B29,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2050,7 +2039,7 @@
       </c>
       <c r="L29" t="str">
         <f>LOOKUP(D29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M29" t="str">
         <f>LOOKUP(E29,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2061,7 +2050,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2078,10 +2067,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
@@ -2089,7 +2078,7 @@
       </c>
       <c r="I30" t="str">
         <f>LOOKUP(A30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J30" t="str">
         <f>LOOKUP(B30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2101,7 +2090,7 @@
       </c>
       <c r="L30" t="str">
         <f>LOOKUP(D30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M30" t="str">
         <f>LOOKUP(E30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2112,7 +2101,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2129,10 +2118,10 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
@@ -2140,7 +2129,7 @@
       </c>
       <c r="I31" t="str">
         <f>LOOKUP(A31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J31" t="str">
         <f>LOOKUP(B31,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2152,7 +2141,7 @@
       </c>
       <c r="L31" t="str">
         <f>LOOKUP(D31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M31" t="str">
         <f>LOOKUP(E31,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2163,7 +2152,7 @@
         <v>constant</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2180,10 +2169,10 @@
         <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
@@ -2191,7 +2180,7 @@
       </c>
       <c r="I32" t="str">
         <f>LOOKUP(A32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J32" t="str">
         <f>LOOKUP(B32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2203,7 +2192,7 @@
       </c>
       <c r="L32" t="str">
         <f>LOOKUP(D32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M32" t="str">
         <f>LOOKUP(E32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2214,7 +2203,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -2231,10 +2220,10 @@
         <v>23</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
@@ -2242,7 +2231,7 @@
       </c>
       <c r="I33" t="str">
         <f>LOOKUP(A33,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J33" t="str">
         <f>LOOKUP(B33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2265,7 +2254,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2282,10 +2271,10 @@
         <v>23</v>
       </c>
       <c r="F34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
@@ -2293,7 +2282,7 @@
       </c>
       <c r="I34" t="str">
         <f>LOOKUP(A34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J34" t="str">
         <f>LOOKUP(B34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2305,7 +2294,7 @@
       </c>
       <c r="L34" t="str">
         <f>LOOKUP(D34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M34" t="str">
         <f>LOOKUP(E34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2316,7 +2305,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2333,10 +2322,10 @@
         <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
@@ -2344,7 +2333,7 @@
       </c>
       <c r="I35" t="str">
         <f>LOOKUP(A35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J35" t="str">
         <f>LOOKUP(B35,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2356,7 +2345,7 @@
       </c>
       <c r="L35" t="str">
         <f>LOOKUP(D35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M35" t="str">
         <f>LOOKUP(E35,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2367,7 +2356,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2384,10 +2373,10 @@
         <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
@@ -2395,7 +2384,7 @@
       </c>
       <c r="I36" t="str">
         <f>LOOKUP(A36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J36" t="str">
         <f>LOOKUP(B36,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2418,7 +2407,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2435,10 +2424,10 @@
         <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
@@ -2446,7 +2435,7 @@
       </c>
       <c r="I37" t="str">
         <f>LOOKUP(A37,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J37" t="str">
         <f>LOOKUP(B37,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2458,7 +2447,7 @@
       </c>
       <c r="L37" t="str">
         <f>LOOKUP(D37,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M37" t="str">
         <f>LOOKUP(E37,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2469,7 +2458,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2486,10 +2475,10 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
@@ -2497,7 +2486,7 @@
       </c>
       <c r="I38" t="str">
         <f>LOOKUP(A38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J38" t="str">
         <f>LOOKUP(B38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2509,7 +2498,7 @@
       </c>
       <c r="L38" t="str">
         <f>LOOKUP(D38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M38" t="str">
         <f>LOOKUP(E38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2520,7 +2509,7 @@
         <v>contrast</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2537,10 +2526,10 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
@@ -2548,7 +2537,7 @@
       </c>
       <c r="I39" t="str">
         <f>LOOKUP(A39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J39" t="str">
         <f>LOOKUP(B39,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2560,7 +2549,7 @@
       </c>
       <c r="L39" t="str">
         <f>LOOKUP(D39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; .5surv length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M39" t="str">
         <f>LOOKUP(E39,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2583,10 +2572,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2647,7 +2636,7 @@
         <v>A30</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2662,12 +2651,12 @@
         <v>A31</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2682,7 +2671,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -2697,7 +2686,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -2712,7 +2701,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2727,7 +2716,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -2742,7 +2731,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>20</v>
@@ -2757,7 +2746,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2767,12 +2756,12 @@
         <v>E0</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2782,12 +2771,12 @@
         <v>E1</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -2797,12 +2786,12 @@
         <v>E2</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2812,12 +2801,12 @@
         <v>F0</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2827,12 +2816,12 @@
         <v>F1</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2842,12 +2831,12 @@
         <v>F2</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -2862,7 +2851,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19">
         <v>30</v>
@@ -2872,12 +2861,12 @@
         <v>L30</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>31</v>
@@ -2887,7 +2876,7 @@
         <v>L31</v>
       </c>
       <c r="D20" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2903,14 +2892,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2918,7 +2907,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2926,7 +2915,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2934,7 +2923,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2942,7 +2931,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change comment in scenarios.xlsx
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Save scenarios.xlsx</t>
   </si>
   <si>
-    <t>Save as scenarios.csv</t>
-  </si>
-  <si>
     <t>Exit</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>I0</t>
+  </si>
+  <si>
+    <t>Run make</t>
   </si>
 </sst>
 </file>
@@ -562,9 +562,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
         <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
@@ -619,7 +619,7 @@
         <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -639,10 +639,10 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE(A2,"-",B2,"-",C2,"-",D2,"-",E2,"-",F2,"-",G2,"-")</f>
@@ -690,10 +690,10 @@
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H28" si="0">CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -792,10 +792,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -843,10 +843,10 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -894,10 +894,10 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -945,10 +945,10 @@
         <v>19</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -996,10 +996,10 @@
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1047,10 +1047,10 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1098,10 +1098,10 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1149,10 +1149,10 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1200,10 +1200,10 @@
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1251,10 +1251,10 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1302,10 +1302,10 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1353,10 +1353,10 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1404,10 +1404,10 @@
         <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -1455,10 +1455,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -1506,10 +1506,10 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1557,10 +1557,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -1608,10 +1608,10 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1659,10 +1659,10 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1710,10 +1710,10 @@
         <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1761,10 +1761,10 @@
         <v>19</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1812,10 +1812,10 @@
         <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -1863,10 +1863,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -1914,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -1965,10 +1965,10 @@
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -2016,10 +2016,10 @@
         <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" ref="H29:H39" si="1">CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
@@ -2067,10 +2067,10 @@
         <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
@@ -2118,10 +2118,10 @@
         <v>3</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="1"/>
@@ -2169,10 +2169,10 @@
         <v>23</v>
       </c>
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="1"/>
@@ -2220,10 +2220,10 @@
         <v>23</v>
       </c>
       <c r="F33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="1"/>
@@ -2271,10 +2271,10 @@
         <v>23</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="1"/>
@@ -2322,10 +2322,10 @@
         <v>19</v>
       </c>
       <c r="F35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="1"/>
@@ -2373,10 +2373,10 @@
         <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="1"/>
@@ -2424,10 +2424,10 @@
         <v>19</v>
       </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="1"/>
@@ -2475,10 +2475,10 @@
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="1"/>
@@ -2526,10 +2526,10 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="1"/>
@@ -2561,7 +2561,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N39"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2791,7 +2790,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2801,12 +2800,12 @@
         <v>F0</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2816,12 +2815,12 @@
         <v>F1</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -2831,7 +2830,7 @@
         <v>F2</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2888,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2923,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2931,7 +2930,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cases of CV
Internally estimate CV while externally estimate the three remaining
growth parameters.
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="74">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -208,6 +208,39 @@
   </si>
   <si>
     <t>Run make</t>
+  </si>
+  <si>
+    <t>A10-C0-D10-L10-E2-F0-I0-</t>
+  </si>
+  <si>
+    <t>A10-C0-D10-L10-E2-F1-I0-</t>
+  </si>
+  <si>
+    <t>A10-C0-D10-L30-E2-F0-I0-</t>
+  </si>
+  <si>
+    <t>A10-C0-D10-L30-E2-F1-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D10-L10-E2-F0-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D10-L10-E2-F1-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D10-L30-E2-F0-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D20-L30-E2-F0-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D10-L30-E2-F1-I0-</t>
+  </si>
+  <si>
+    <t>A30-C0-D20-L30-E2-F1-I0-</t>
+  </si>
+  <si>
+    <t>E3</t>
   </si>
 </sst>
 </file>
@@ -560,9 +593,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
@@ -684,10 +717,10 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -696,8 +729,8 @@
         <v>61</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H28" si="0">CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
-        <v>A0-C0-D0-L30-E0-F0-I0-</v>
+        <f>CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
+        <v>A0-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I3" t="str">
         <f>LOOKUP(A3,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -713,11 +746,11 @@
       </c>
       <c r="L3" t="str">
         <f>LOOKUP(D3,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M3" t="str">
         <f>LOOKUP(E3,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N3" t="str">
         <f>LOOKUP(F3,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -726,7 +759,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -738,7 +771,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -747,12 +780,12 @@
         <v>61</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E1-F0-I0-</v>
+        <f>CONCATENATE(A4,"-",B4,"-",C4,"-",D4,"-",E4,"-",F4,"-",G4,"-")</f>
+        <v>A10-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I4" t="str">
         <f>LOOKUP(A4,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish age</v>
       </c>
       <c r="J4" t="str">
         <f>LOOKUP(B4,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -768,7 +801,7 @@
       </c>
       <c r="M4" t="str">
         <f>LOOKUP(E4,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N4" t="str">
         <f>LOOKUP(F4,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -777,7 +810,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -786,7 +819,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -798,12 +831,12 @@
         <v>61</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L30-E1-F0-I0-</v>
+        <f>CONCATENATE(A5,"-",B5,"-",C5,"-",D5,"-",E5,"-",F5,"-",G5,"-")</f>
+        <v>A10-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I5" t="str">
         <f>LOOKUP(A5,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish age</v>
       </c>
       <c r="J5" t="str">
         <f>LOOKUP(B5,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -815,7 +848,7 @@
       </c>
       <c r="L5" t="str">
         <f>LOOKUP(D5,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M5" t="str">
         <f>LOOKUP(E5,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -828,33 +861,33 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>61</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E0-F1-I0-</v>
+        <f>CONCATENATE(A6,"-",B6,"-",C6,"-",D6,"-",E6,"-",F6,"-",G6,"-")</f>
+        <v>A10-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I6" t="str">
         <f>LOOKUP(A6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish age</v>
       </c>
       <c r="J6" t="str">
         <f>LOOKUP(B6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -862,7 +895,7 @@
       </c>
       <c r="K6" t="str">
         <f>LOOKUP(C6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L6" t="str">
         <f>LOOKUP(D6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -870,67 +903,60 @@
       </c>
       <c r="M6" t="str">
         <f>LOOKUP(E6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>external</v>
       </c>
       <c r="N6" t="str">
         <f>LOOKUP(F6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
         <v>61</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L30-E0-F1-I0-</v>
-      </c>
-      <c r="I7" t="str">
-        <f>LOOKUP(A7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
-      </c>
-      <c r="J7" t="str">
-        <f>LOOKUP(B7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K7" t="str">
-        <f>LOOKUP(C7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L7" t="str">
-        <f>LOOKUP(D7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M7" t="str">
-        <f>LOOKUP(E7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
-      </c>
-      <c r="N7" t="str">
-        <f>LOOKUP(F7,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -942,21 +968,21 @@
         <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
         <v>61</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E1-F1-I0-</v>
+        <f>CONCATENATE(A8,"-",B8,"-",C8,"-",D8,"-",E8,"-",F8,"-",G8,"-")</f>
+        <v>A30-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I8" t="str">
         <f>LOOKUP(A8,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J8" t="str">
         <f>LOOKUP(B8,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -972,16 +998,16 @@
       </c>
       <c r="M8" t="str">
         <f>LOOKUP(E8,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N8" t="str">
         <f>LOOKUP(F8,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -990,24 +1016,24 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
         <v>61</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>A0-C0-D0-L30-E1-F1-I0-</v>
+        <f>CONCATENATE(A9,"-",B9,"-",C9,"-",D9,"-",E9,"-",F9,"-",G9,"-")</f>
+        <v>A30-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I9" t="str">
         <f>LOOKUP(A9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J9" t="str">
         <f>LOOKUP(B9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1019,7 +1045,7 @@
       </c>
       <c r="L9" t="str">
         <f>LOOKUP(D9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M9" t="str">
         <f>LOOKUP(E9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1027,24 +1053,24 @@
       </c>
       <c r="N9" t="str">
         <f>LOOKUP(F9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
@@ -1053,12 +1079,12 @@
         <v>61</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E0-F0-I0-</v>
+        <f>CONCATENATE(A10,"-",B10,"-",C10,"-",D10,"-",E10,"-",F10,"-",G10,"-")</f>
+        <v>A30-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I10" t="str">
         <f>LOOKUP(A10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J10" t="str">
         <f>LOOKUP(B10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1066,7 +1092,7 @@
       </c>
       <c r="K10" t="str">
         <f>LOOKUP(C10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L10" t="str">
         <f>LOOKUP(D10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1074,7 +1100,7 @@
       </c>
       <c r="M10" t="str">
         <f>LOOKUP(E10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>external</v>
       </c>
       <c r="N10" t="str">
         <f>LOOKUP(F10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1083,19 +1109,19 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
@@ -1103,38 +1129,31 @@
       <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L30-E0-F0-I0-</v>
-      </c>
-      <c r="I11" t="str">
-        <f>LOOKUP(A11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J11" t="str">
-        <f>LOOKUP(B11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K11" t="str">
-        <f>LOOKUP(C11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L11" t="str">
-        <f>LOOKUP(D11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M11" t="str">
-        <f>LOOKUP(E11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
-      </c>
-      <c r="N11" t="str">
-        <f>LOOKUP(F11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1143,10 +1162,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
@@ -1155,12 +1174,12 @@
         <v>61</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E1-F0-I0-</v>
+        <f>CONCATENATE(A12,"-",B12,"-",C12,"-",D12,"-",E12,"-",F12,"-",G12,"-")</f>
+        <v>A0-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I12" t="str">
         <f>LOOKUP(A12,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>no age</v>
       </c>
       <c r="J12" t="str">
         <f>LOOKUP(B12,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1172,11 +1191,11 @@
       </c>
       <c r="L12" t="str">
         <f>LOOKUP(D12,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M12" t="str">
         <f>LOOKUP(E12,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N12" t="str">
         <f>LOOKUP(F12,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1185,7 +1204,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -1206,12 +1225,12 @@
         <v>61</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L30-E1-F0-I0-</v>
+        <f>CONCATENATE(A13,"-",B13,"-",C13,"-",D13,"-",E13,"-",F13,"-",G13,"-")</f>
+        <v>A0-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I13" t="str">
         <f>LOOKUP(A13,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>no age</v>
       </c>
       <c r="J13" t="str">
         <f>LOOKUP(B13,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1245,20 +1264,20 @@
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
         <v>61</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E0-F1-I0-</v>
+        <f>CONCATENATE(A14,"-",B14,"-",C14,"-",D14,"-",E14,"-",F14,"-",G14,"-")</f>
+        <v>A10-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I14" t="str">
         <f>LOOKUP(A14,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1274,7 +1293,7 @@
       </c>
       <c r="L14" t="str">
         <f>LOOKUP(D14,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M14" t="str">
         <f>LOOKUP(E14,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1282,7 +1301,7 @@
       </c>
       <c r="N14" t="str">
         <f>LOOKUP(F14,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1299,17 +1318,17 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
         <v>61</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L30-E0-F1-I0-</v>
+        <f>CONCATENATE(A15,"-",B15,"-",C15,"-",D15,"-",E15,"-",F15,"-",G15,"-")</f>
+        <v>A10-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I15" t="str">
         <f>LOOKUP(A15,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1329,11 +1348,11 @@
       </c>
       <c r="M15" t="str">
         <f>LOOKUP(E15,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N15" t="str">
         <f>LOOKUP(F15,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1344,23 +1363,23 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
         <v>61</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E1-F1-I0-</v>
+        <f>CONCATENATE(A16,"-",B16,"-",C16,"-",D16,"-",E16,"-",F16,"-",G16,"-")</f>
+        <v>A10-C0-D10-L30-E2-F0-I0-</v>
       </c>
       <c r="I16" t="str">
         <f>LOOKUP(A16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1372,19 +1391,19 @@
       </c>
       <c r="K16" t="str">
         <f>LOOKUP(C16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L16" t="str">
         <f>LOOKUP(D16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M16" t="str">
         <f>LOOKUP(E16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>external</v>
       </c>
       <c r="N16" t="str">
         <f>LOOKUP(F16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1395,64 +1414,57 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" t="s">
         <v>61</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L30-E1-F1-I0-</v>
-      </c>
-      <c r="I17" t="str">
-        <f>LOOKUP(A17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J17" t="str">
-        <f>LOOKUP(B17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K17" t="str">
-        <f>LOOKUP(C17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L17" t="str">
-        <f>LOOKUP(D17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M17" t="str">
-        <f>LOOKUP(E17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
-      </c>
-      <c r="N17" t="str">
-        <f>LOOKUP(F17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
         <v>54</v>
@@ -1461,12 +1473,12 @@
         <v>61</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E2-F0-I0-</v>
+        <f>CONCATENATE(A18,"-",B18,"-",C18,"-",D18,"-",E18,"-",F18,"-",G18,"-")</f>
+        <v>A30-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I18" t="str">
         <f>LOOKUP(A18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J18" t="str">
         <f>LOOKUP(B18,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1474,15 +1486,15 @@
       </c>
       <c r="K18" t="str">
         <f>LOOKUP(C18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L18" t="str">
         <f>LOOKUP(D18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M18" t="str">
         <f>LOOKUP(E18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>fixed</v>
       </c>
       <c r="N18" t="str">
         <f>LOOKUP(F18,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1491,33 +1503,33 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" t="s">
         <v>61</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E2-F1-I0-</v>
+        <f>CONCATENATE(A19,"-",B19,"-",C19,"-",D19,"-",E19,"-",F19,"-",G19,"-")</f>
+        <v>A30-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I19" t="str">
         <f>LOOKUP(A19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J19" t="str">
         <f>LOOKUP(B19,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1525,36 +1537,36 @@
       </c>
       <c r="K19" t="str">
         <f>LOOKUP(C19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L19" t="str">
         <f>LOOKUP(D19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M19" t="str">
         <f>LOOKUP(E19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>internal</v>
       </c>
       <c r="N19" t="str">
         <f>LOOKUP(F19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F20" t="s">
         <v>54</v>
@@ -1563,20 +1575,20 @@
         <v>61</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L30-E2-F0-I0-</v>
+        <f>CONCATENATE(A20,"-",B20,"-",C20,"-",D20,"-",E20,"-",F20,"-",G20,"-")</f>
+        <v>A30-C20-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I20" t="str">
         <f>LOOKUP(A20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J20" t="str">
         <f>LOOKUP(B20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K20" t="str">
         <f>LOOKUP(C20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L20" t="str">
         <f>LOOKUP(D20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1584,7 +1596,7 @@
       </c>
       <c r="M20" t="str">
         <f>LOOKUP(E20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>fixed</v>
       </c>
       <c r="N20" t="str">
         <f>LOOKUP(F20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1593,41 +1605,41 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
         <v>61</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L30-E2-F1-I0-</v>
+        <f>CONCATENATE(A21,"-",B21,"-",C21,"-",D21,"-",E21,"-",F21,"-",G21,"-")</f>
+        <v>A30-C20-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I21" t="str">
         <f>LOOKUP(A21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J21" t="str">
         <f>LOOKUP(B21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K21" t="str">
         <f>LOOKUP(C21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L21" t="str">
         <f>LOOKUP(D21,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1635,11 +1647,11 @@
       </c>
       <c r="M21" t="str">
         <f>LOOKUP(E21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>internal</v>
       </c>
       <c r="N21" t="str">
         <f>LOOKUP(F21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+        <v>constant</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1650,13 +1662,13 @@
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -1665,8 +1677,8 @@
         <v>61</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D0-L10-E0-F0-I0-</v>
+        <f>CONCATENATE(A22,"-",B22,"-",C22,"-",D22,"-",E22,"-",F22,"-",G22,"-")</f>
+        <v>A30-C0-D10-L30-E2-F0-I0-</v>
       </c>
       <c r="I22" t="str">
         <f>LOOKUP(A22,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1678,15 +1690,15 @@
       </c>
       <c r="K22" t="str">
         <f>LOOKUP(C22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L22" t="str">
         <f>LOOKUP(D22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M22" t="str">
         <f>LOOKUP(E22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>external</v>
       </c>
       <c r="N22" t="str">
         <f>LOOKUP(F22,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1701,13 +1713,13 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
         <v>54</v>
@@ -1715,33 +1727,26 @@
       <c r="G23" t="s">
         <v>61</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D0-L30-E0-F0-I0-</v>
-      </c>
-      <c r="I23" t="str">
-        <f>LOOKUP(A23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J23" t="str">
-        <f>LOOKUP(B23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K23" t="str">
-        <f>LOOKUP(C23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L23" t="str">
-        <f>LOOKUP(D23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M23" t="str">
-        <f>LOOKUP(E23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
-      </c>
-      <c r="N23" t="str">
-        <f>LOOKUP(F23,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>48</v>
+      </c>
+      <c r="N23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1752,13 +1757,13 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>54</v>
@@ -1767,8 +1772,8 @@
         <v>61</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D0-L10-E1-F0-I0-</v>
+        <f>CONCATENATE(A24,"-",B24,"-",C24,"-",D24,"-",E24,"-",F24,"-",G24,"-")</f>
+        <v>A30-C0-D20-L30-E2-F0-I0-</v>
       </c>
       <c r="I24" t="str">
         <f>LOOKUP(A24,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1780,15 +1785,15 @@
       </c>
       <c r="K24" t="str">
         <f>LOOKUP(C24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>surv mlacomp</v>
       </c>
       <c r="L24" t="str">
         <f>LOOKUP(D24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M24" t="str">
         <f>LOOKUP(E24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>external</v>
       </c>
       <c r="N24" t="str">
         <f>LOOKUP(F24,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1803,13 +1808,13 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F25" t="s">
         <v>54</v>
@@ -1817,64 +1822,57 @@
       <c r="G25" t="s">
         <v>61</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D0-L30-E1-F0-I0-</v>
-      </c>
-      <c r="I25" t="str">
-        <f>LOOKUP(A25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J25" t="str">
-        <f>LOOKUP(B25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K25" t="str">
-        <f>LOOKUP(C25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L25" t="str">
-        <f>LOOKUP(D25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M25" t="str">
-        <f>LOOKUP(E25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
-      </c>
-      <c r="N25" t="str">
-        <f>LOOKUP(F25,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" t="s">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
         <v>61</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D10-L10-E2-F0-I0-</v>
+        <f>CONCATENATE(A26,"-",B26,"-",C26,"-",D26,"-",E26,"-",F26,"-",G26,"-")</f>
+        <v>A0-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I26" t="str">
         <f>LOOKUP(A26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J26" t="str">
         <f>LOOKUP(B26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1882,7 +1880,7 @@
       </c>
       <c r="K26" t="str">
         <f>LOOKUP(C26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L26" t="str">
         <f>LOOKUP(D26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1890,28 +1888,28 @@
       </c>
       <c r="M26" t="str">
         <f>LOOKUP(E26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>fixed</v>
       </c>
       <c r="N26" t="str">
         <f>LOOKUP(F26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+        <v>contrast</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F27" t="s">
         <v>55</v>
@@ -1920,12 +1918,12 @@
         <v>61</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D10-L10-E2-F1-I0-</v>
+        <f>CONCATENATE(A27,"-",B27,"-",C27,"-",D27,"-",E27,"-",F27,"-",G27,"-")</f>
+        <v>A0-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I27" t="str">
         <f>LOOKUP(A27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J27" t="str">
         <f>LOOKUP(B27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1933,7 +1931,7 @@
       </c>
       <c r="K27" t="str">
         <f>LOOKUP(C27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L27" t="str">
         <f>LOOKUP(D27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1941,7 +1939,7 @@
       </c>
       <c r="M27" t="str">
         <f>LOOKUP(E27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>internal</v>
       </c>
       <c r="N27" t="str">
         <f>LOOKUP(F27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1950,33 +1948,33 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
         <v>61</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v>A30-C0-D10-L30-E2-F0-I0-</v>
+        <f>CONCATENATE(A28,"-",B28,"-",C28,"-",D28,"-",E28,"-",F28,"-",G28,"-")</f>
+        <v>A10-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I28" t="str">
         <f>LOOKUP(A28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J28" t="str">
         <f>LOOKUP(B28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1984,54 +1982,54 @@
       </c>
       <c r="K28" t="str">
         <f>LOOKUP(C28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L28" t="str">
         <f>LOOKUP(D28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M28" t="str">
         <f>LOOKUP(E28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>fixed</v>
       </c>
       <c r="N28" t="str">
         <f>LOOKUP(F28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+        <v>contrast</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
         <v>61</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" ref="H29:H39" si="1">CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
-        <v>A30-C20-D0-L30-E0-F0-I0-</v>
+        <f>CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
+        <v>A10-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I29" t="str">
         <f>LOOKUP(A29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J29" t="str">
         <f>LOOKUP(B29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K29" t="str">
         <f>LOOKUP(C29,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2039,117 +2037,110 @@
       </c>
       <c r="L29" t="str">
         <f>LOOKUP(D29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M29" t="str">
         <f>LOOKUP(E29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N29" t="str">
         <f>LOOKUP(F29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+        <v>contrast</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
         <v>61</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C20-D0-L30-E1-F0-I0-</v>
+        <f>CONCATENATE(A30,"-",B30,"-",C30,"-",D30,"-",E30,"-",F30,"-",G30,"-")</f>
+        <v>A10-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I30" t="str">
         <f>LOOKUP(A30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J30" t="str">
         <f>LOOKUP(B30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K30" t="str">
         <f>LOOKUP(C30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L30" t="str">
         <f>LOOKUP(D30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M30" t="str">
         <f>LOOKUP(E30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>external</v>
       </c>
       <c r="N30" t="str">
         <f>LOOKUP(F30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+        <v>contrast</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
         <v>61</v>
       </c>
-      <c r="H31" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D20-L30-E2-F0-I0-</v>
-      </c>
-      <c r="I31" t="str">
-        <f>LOOKUP(A31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J31" t="str">
-        <f>LOOKUP(B31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K31" t="str">
-        <f>LOOKUP(C31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv mlacomp</v>
-      </c>
-      <c r="L31" t="str">
-        <f>LOOKUP(D31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M31" t="str">
-        <f>LOOKUP(E31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
-      </c>
-      <c r="N31" t="str">
-        <f>LOOKUP(F31,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" t="s">
+        <v>48</v>
+      </c>
+      <c r="N31" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2157,13 +2148,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
         <v>23</v>
@@ -2175,8 +2166,8 @@
         <v>61</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C20-D0-L30-E0-F1-I0-</v>
+        <f>CONCATENATE(A32,"-",B32,"-",C32,"-",D32,"-",E32,"-",F32,"-",G32,"-")</f>
+        <v>A30-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I32" t="str">
         <f>LOOKUP(A32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2184,7 +2175,7 @@
       </c>
       <c r="J32" t="str">
         <f>LOOKUP(B32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K32" t="str">
         <f>LOOKUP(C32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2192,7 +2183,7 @@
       </c>
       <c r="L32" t="str">
         <f>LOOKUP(D32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M32" t="str">
         <f>LOOKUP(E32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2217,7 +2208,7 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
@@ -2226,8 +2217,8 @@
         <v>61</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D0-L10-E0-F1-I0-</v>
+        <f>CONCATENATE(A33,"-",B33,"-",C33,"-",D33,"-",E33,"-",F33,"-",G33,"-")</f>
+        <v>A30-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I33" t="str">
         <f>LOOKUP(A33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2247,7 +2238,7 @@
       </c>
       <c r="M33" t="str">
         <f>LOOKUP(E33,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N33" t="str">
         <f>LOOKUP(F33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2262,13 +2253,13 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
         <v>55</v>
@@ -2277,8 +2268,8 @@
         <v>61</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D0-L30-E0-F1-I0-</v>
+        <f>CONCATENATE(A34,"-",B34,"-",C34,"-",D34,"-",E34,"-",F34,"-",G34,"-")</f>
+        <v>A30-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I34" t="str">
         <f>LOOKUP(A34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2290,15 +2281,15 @@
       </c>
       <c r="K34" t="str">
         <f>LOOKUP(C34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L34" t="str">
         <f>LOOKUP(D34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M34" t="str">
         <f>LOOKUP(E34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>external</v>
       </c>
       <c r="N34" t="str">
         <f>LOOKUP(F34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2310,16 +2301,16 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F35" t="s">
         <v>55</v>
@@ -2327,38 +2318,31 @@
       <c r="G35" t="s">
         <v>61</v>
       </c>
-      <c r="H35" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C20-D0-L30-E1-F1-I0-</v>
-      </c>
-      <c r="I35" t="str">
-        <f>LOOKUP(A35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J35" t="str">
-        <f>LOOKUP(B35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
-      </c>
-      <c r="K35" t="str">
-        <f>LOOKUP(C35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L35" t="str">
-        <f>LOOKUP(D35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M35" t="str">
-        <f>LOOKUP(E35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
-      </c>
-      <c r="N35" t="str">
-        <f>LOOKUP(F35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" t="s">
+        <v>48</v>
+      </c>
+      <c r="N35" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
@@ -2367,10 +2351,10 @@
         <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F36" t="s">
         <v>55</v>
@@ -2379,12 +2363,12 @@
         <v>61</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D0-L10-E1-F1-I0-</v>
+        <f>CONCATENATE(A36,"-",B36,"-",C36,"-",D36,"-",E36,"-",F36,"-",G36,"-")</f>
+        <v>A0-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I36" t="str">
         <f>LOOKUP(A36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J36" t="str">
         <f>LOOKUP(B36,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2396,11 +2380,11 @@
       </c>
       <c r="L36" t="str">
         <f>LOOKUP(D36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M36" t="str">
         <f>LOOKUP(E36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N36" t="str">
         <f>LOOKUP(F36,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2409,7 +2393,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -2430,12 +2414,12 @@
         <v>61</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D0-L30-E1-F1-I0-</v>
+        <f>CONCATENATE(A37,"-",B37,"-",C37,"-",D37,"-",E37,"-",F37,"-",G37,"-")</f>
+        <v>A0-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I37" t="str">
         <f>LOOKUP(A37,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J37" t="str">
         <f>LOOKUP(B37,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2460,19 +2444,19 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F38" t="s">
         <v>55</v>
@@ -2481,12 +2465,12 @@
         <v>61</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D10-L30-E2-F1-I0-</v>
+        <f>CONCATENATE(A38,"-",B38,"-",C38,"-",D38,"-",E38,"-",F38,"-",G38,"-")</f>
+        <v>A10-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I38" t="str">
         <f>LOOKUP(A38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J38" t="str">
         <f>LOOKUP(B38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2494,7 +2478,7 @@
       </c>
       <c r="K38" t="str">
         <f>LOOKUP(C38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L38" t="str">
         <f>LOOKUP(D38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2502,7 +2486,7 @@
       </c>
       <c r="M38" t="str">
         <f>LOOKUP(E38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>fixed</v>
       </c>
       <c r="N38" t="str">
         <f>LOOKUP(F38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2511,19 +2495,19 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F39" t="s">
         <v>55</v>
@@ -2532,12 +2516,12 @@
         <v>61</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="1"/>
-        <v>A30-C0-D20-L30-E2-F1-I0-</v>
+        <f>CONCATENATE(A39,"-",B39,"-",C39,"-",D39,"-",E39,"-",F39,"-",G39,"-")</f>
+        <v>A10-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I39" t="str">
         <f>LOOKUP(A39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J39" t="str">
         <f>LOOKUP(B39,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2545,7 +2529,7 @@
       </c>
       <c r="K39" t="str">
         <f>LOOKUP(C39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L39" t="str">
         <f>LOOKUP(D39,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2553,14 +2537,511 @@
       </c>
       <c r="M39" t="str">
         <f>LOOKUP(E39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>internal</v>
       </c>
       <c r="N39" t="str">
         <f>LOOKUP(F39,descriptions!$C:$C,descriptions!$D:$D)</f>
         <v>contrast</v>
       </c>
     </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G40" t="s">
+        <v>61</v>
+      </c>
+      <c r="H40" t="str">
+        <f>CONCATENATE(A40,"-",B40,"-",C40,"-",D40,"-",E40,"-",F40,"-",G40,"-")</f>
+        <v>A10-C0-D10-L30-E2-F1-I0-</v>
+      </c>
+      <c r="I40" t="str">
+        <f>LOOKUP(A40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J40" t="str">
+        <f>LOOKUP(B40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K40" t="str">
+        <f>LOOKUP(C40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L40" t="str">
+        <f>LOOKUP(D40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M40" t="str">
+        <f>LOOKUP(E40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>external</v>
+      </c>
+      <c r="N40" t="str">
+        <f>LOOKUP(F40,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" t="s">
+        <v>61</v>
+      </c>
+      <c r="H41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>48</v>
+      </c>
+      <c r="N41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" t="str">
+        <f>CONCATENATE(A42,"-",B42,"-",C42,"-",D42,"-",E42,"-",F42,"-",G42,"-")</f>
+        <v>A30-C0-D0-L30-E0-F1-I0-</v>
+      </c>
+      <c r="I42" t="str">
+        <f>LOOKUP(A42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J42" t="str">
+        <f>LOOKUP(B42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K42" t="str">
+        <f>LOOKUP(C42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L42" t="str">
+        <f>LOOKUP(D42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M42" t="str">
+        <f>LOOKUP(E42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fixed</v>
+      </c>
+      <c r="N42" t="str">
+        <f>LOOKUP(F42,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H43" t="str">
+        <f>CONCATENATE(A43,"-",B43,"-",C43,"-",D43,"-",E43,"-",F43,"-",G43,"-")</f>
+        <v>A30-C0-D0-L30-E1-F1-I0-</v>
+      </c>
+      <c r="I43" t="str">
+        <f>LOOKUP(A43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J43" t="str">
+        <f>LOOKUP(B43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K43" t="str">
+        <f>LOOKUP(C43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L43" t="str">
+        <f>LOOKUP(D43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M43" t="str">
+        <f>LOOKUP(E43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>internal</v>
+      </c>
+      <c r="N43" t="str">
+        <f>LOOKUP(F43,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" t="s">
+        <v>55</v>
+      </c>
+      <c r="G44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H44" t="str">
+        <f>CONCATENATE(A44,"-",B44,"-",C44,"-",D44,"-",E44,"-",F44,"-",G44,"-")</f>
+        <v>A30-C20-D0-L30-E0-F1-I0-</v>
+      </c>
+      <c r="I44" t="str">
+        <f>LOOKUP(A44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J44" t="str">
+        <f>LOOKUP(B44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>surv calcomp</v>
+      </c>
+      <c r="K44" t="str">
+        <f>LOOKUP(C44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L44" t="str">
+        <f>LOOKUP(D44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M44" t="str">
+        <f>LOOKUP(E44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fixed</v>
+      </c>
+      <c r="N44" t="str">
+        <f>LOOKUP(F44,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" t="str">
+        <f>CONCATENATE(A45,"-",B45,"-",C45,"-",D45,"-",E45,"-",F45,"-",G45,"-")</f>
+        <v>A30-C20-D0-L30-E1-F1-I0-</v>
+      </c>
+      <c r="I45" t="str">
+        <f>LOOKUP(A45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J45" t="str">
+        <f>LOOKUP(B45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>surv calcomp</v>
+      </c>
+      <c r="K45" t="str">
+        <f>LOOKUP(C45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L45" t="str">
+        <f>LOOKUP(D45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M45" t="str">
+        <f>LOOKUP(E45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>internal</v>
+      </c>
+      <c r="N45" t="str">
+        <f>LOOKUP(F45,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>55</v>
+      </c>
+      <c r="G46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" t="str">
+        <f>CONCATENATE(A46,"-",B46,"-",C46,"-",D46,"-",E46,"-",F46,"-",G46,"-")</f>
+        <v>A30-C0-D10-L30-E2-F1-I0-</v>
+      </c>
+      <c r="I46" t="str">
+        <f>LOOKUP(A46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J46" t="str">
+        <f>LOOKUP(B46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K46" t="str">
+        <f>LOOKUP(C46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L46" t="str">
+        <f>LOOKUP(D46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M46" t="str">
+        <f>LOOKUP(E46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>external</v>
+      </c>
+      <c r="N46" t="str">
+        <f>LOOKUP(F46,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" t="s">
+        <v>61</v>
+      </c>
+      <c r="H47" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" t="s">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>48</v>
+      </c>
+      <c r="N47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" t="str">
+        <f>CONCATENATE(A48,"-",B48,"-",C48,"-",D48,"-",E48,"-",F48,"-",G48,"-")</f>
+        <v>A30-C0-D20-L30-E2-F1-I0-</v>
+      </c>
+      <c r="I48" t="str">
+        <f>LOOKUP(A48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J48" t="str">
+        <f>LOOKUP(B48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K48" t="str">
+        <f>LOOKUP(C48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>surv mlacomp</v>
+      </c>
+      <c r="L48" t="str">
+        <f>LOOKUP(D48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M48" t="str">
+        <f>LOOKUP(E48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>external</v>
+      </c>
+      <c r="N48" t="str">
+        <f>LOOKUP(F48,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+      <c r="F49" t="s">
+        <v>55</v>
+      </c>
+      <c r="G49" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" t="s">
+        <v>72</v>
+      </c>
+      <c r="I49" t="s">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>12</v>
+      </c>
+      <c r="K49" t="s">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>48</v>
+      </c>
+      <c r="N49" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:N49">
+    <sortCondition ref="F2:F49"/>
+    <sortCondition ref="D2:D49"/>
+    <sortCondition ref="A2:A49"/>
+    <sortCondition ref="C2:C49"/>
+    <sortCondition ref="B2:B49"/>
+    <sortCondition ref="E2:E49"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2887,7 +3368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add M misspecification and fix bug
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -12,14 +12,14 @@
     <sheet name="readme" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$49</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="95">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -241,6 +241,69 @@
   </si>
   <si>
     <t>E3</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>E18</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>internalCV</t>
+  </si>
+  <si>
+    <t>M60</t>
+  </si>
+  <si>
+    <t>M80</t>
+  </si>
+  <si>
+    <t>M50</t>
+  </si>
+  <si>
+    <t>M70</t>
+  </si>
+  <si>
+    <t>M90</t>
+  </si>
+  <si>
+    <t>M110</t>
+  </si>
+  <si>
+    <t>M120</t>
+  </si>
+  <si>
+    <t>M130</t>
+  </si>
+  <si>
+    <t>M140</t>
+  </si>
+  <si>
+    <t>M150</t>
   </si>
 </sst>
 </file>
@@ -593,11 +656,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +966,7 @@
       </c>
       <c r="M6" t="str">
         <f>LOOKUP(E6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N6" t="str">
         <f>LOOKUP(F6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1100,7 +1163,7 @@
       </c>
       <c r="M10" t="str">
         <f>LOOKUP(E10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N10" t="str">
         <f>LOOKUP(F10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1399,7 +1462,7 @@
       </c>
       <c r="M16" t="str">
         <f>LOOKUP(E16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N16" t="str">
         <f>LOOKUP(F16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1698,7 +1761,7 @@
       </c>
       <c r="M22" t="str">
         <f>LOOKUP(E22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N22" t="str">
         <f>LOOKUP(F22,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1793,7 +1856,7 @@
       </c>
       <c r="M24" t="str">
         <f>LOOKUP(E24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N24" t="str">
         <f>LOOKUP(F24,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2092,7 +2155,7 @@
       </c>
       <c r="M30" t="str">
         <f>LOOKUP(E30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N30" t="str">
         <f>LOOKUP(F30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2289,7 +2352,7 @@
       </c>
       <c r="M34" t="str">
         <f>LOOKUP(E34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N34" t="str">
         <f>LOOKUP(F34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2588,7 +2651,7 @@
       </c>
       <c r="M40" t="str">
         <f>LOOKUP(E40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N40" t="str">
         <f>LOOKUP(F40,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2887,7 +2950,7 @@
       </c>
       <c r="M46" t="str">
         <f>LOOKUP(E46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N46" t="str">
         <f>LOOKUP(F46,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2982,7 +3045,7 @@
       </c>
       <c r="M48" t="str">
         <f>LOOKUP(E48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>external</v>
+        <v>M150</v>
       </c>
       <c r="N48" t="str">
         <f>LOOKUP(F48,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3033,7 +3096,1028 @@
         <v>59</v>
       </c>
     </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" t="s">
+        <v>55</v>
+      </c>
+      <c r="G50" t="s">
+        <v>61</v>
+      </c>
+      <c r="H50" t="str">
+        <f>CONCATENATE(A50,"-",B50,"-",C50,"-",D50,"-",E50,"-",F50,"-",G50,"-")</f>
+        <v>A10-C0-D0-L10-E10-F1-I0-</v>
+      </c>
+      <c r="I50" t="str">
+        <f>LOOKUP(A50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J50" t="str">
+        <f>LOOKUP(B50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K50" t="str">
+        <f>LOOKUP(C50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L50" t="str">
+        <f>LOOKUP(D50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M50" t="str">
+        <f>LOOKUP(E50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M50</v>
+      </c>
+      <c r="N50" t="str">
+        <f>LOOKUP(F50,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F51" t="s">
+        <v>55</v>
+      </c>
+      <c r="G51" t="s">
+        <v>61</v>
+      </c>
+      <c r="H51" t="str">
+        <f>CONCATENATE(A51,"-",B51,"-",C51,"-",D51,"-",E51,"-",F51,"-",G51,"-")</f>
+        <v>A10-C0-D10-L10-E10-F1-I0-</v>
+      </c>
+      <c r="I51" t="str">
+        <f>LOOKUP(A51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J51" t="str">
+        <f>LOOKUP(B51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K51" t="str">
+        <f>LOOKUP(C51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L51" t="str">
+        <f>LOOKUP(D51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M51" t="str">
+        <f>LOOKUP(E51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M50</v>
+      </c>
+      <c r="N51" t="str">
+        <f>LOOKUP(F51,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" t="s">
+        <v>55</v>
+      </c>
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" t="str">
+        <f>CONCATENATE(A52,"-",B52,"-",C52,"-",D52,"-",E52,"-",F52,"-",G52,"-")</f>
+        <v>A10-C0-D0-L10-E11-F1-I0-</v>
+      </c>
+      <c r="I52" t="str">
+        <f>LOOKUP(A52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J52" t="str">
+        <f>LOOKUP(B52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K52" t="str">
+        <f>LOOKUP(C52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L52" t="str">
+        <f>LOOKUP(D52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M52" t="str">
+        <f>LOOKUP(E52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M60</v>
+      </c>
+      <c r="N52" t="str">
+        <f>LOOKUP(F52,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>75</v>
+      </c>
+      <c r="F53" t="s">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s">
+        <v>61</v>
+      </c>
+      <c r="H53" t="str">
+        <f>CONCATENATE(A53,"-",B53,"-",C53,"-",D53,"-",E53,"-",F53,"-",G53,"-")</f>
+        <v>A10-C0-D10-L10-E11-F1-I0-</v>
+      </c>
+      <c r="I53" t="str">
+        <f>LOOKUP(A53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J53" t="str">
+        <f>LOOKUP(B53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K53" t="str">
+        <f>LOOKUP(C53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L53" t="str">
+        <f>LOOKUP(D53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M53" t="str">
+        <f>LOOKUP(E53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M60</v>
+      </c>
+      <c r="N53" t="str">
+        <f>LOOKUP(F53,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" t="s">
+        <v>55</v>
+      </c>
+      <c r="G54" t="s">
+        <v>61</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" ref="H54:H69" si="0">CONCATENATE(A54,"-",B54,"-",C54,"-",D54,"-",E54,"-",F54,"-",G54,"-")</f>
+        <v>A10-C0-D0-L10-E12-F1-I0-</v>
+      </c>
+      <c r="I54" t="str">
+        <f>LOOKUP(A54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J54" t="str">
+        <f>LOOKUP(B54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K54" t="str">
+        <f>LOOKUP(C54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L54" t="str">
+        <f>LOOKUP(D54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M54" t="str">
+        <f>LOOKUP(E54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M70</v>
+      </c>
+      <c r="N54" t="str">
+        <f>LOOKUP(F54,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s">
+        <v>76</v>
+      </c>
+      <c r="F55" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" t="s">
+        <v>61</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E12-F1-I0-</v>
+      </c>
+      <c r="I55" t="str">
+        <f>LOOKUP(A55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J55" t="str">
+        <f>LOOKUP(B55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K55" t="str">
+        <f>LOOKUP(C55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L55" t="str">
+        <f>LOOKUP(D55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M55" t="str">
+        <f>LOOKUP(E55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M70</v>
+      </c>
+      <c r="N55" t="str">
+        <f>LOOKUP(F55,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" t="s">
+        <v>55</v>
+      </c>
+      <c r="G56" t="s">
+        <v>61</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E13-F1-I0-</v>
+      </c>
+      <c r="I56" t="str">
+        <f>LOOKUP(A56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J56" t="str">
+        <f>LOOKUP(B56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K56" t="str">
+        <f>LOOKUP(C56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L56" t="str">
+        <f>LOOKUP(D56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M56" t="str">
+        <f>LOOKUP(E56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M80</v>
+      </c>
+      <c r="N56" t="str">
+        <f>LOOKUP(F56,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" t="s">
+        <v>55</v>
+      </c>
+      <c r="G57" t="s">
+        <v>61</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E13-F1-I0-</v>
+      </c>
+      <c r="I57" t="str">
+        <f>LOOKUP(A57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J57" t="str">
+        <f>LOOKUP(B57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K57" t="str">
+        <f>LOOKUP(C57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L57" t="str">
+        <f>LOOKUP(D57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M57" t="str">
+        <f>LOOKUP(E57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M80</v>
+      </c>
+      <c r="N57" t="str">
+        <f>LOOKUP(F57,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
+      </c>
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" t="s">
+        <v>55</v>
+      </c>
+      <c r="G58" t="s">
+        <v>61</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E14-F1-I0-</v>
+      </c>
+      <c r="I58" t="str">
+        <f>LOOKUP(A58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J58" t="str">
+        <f>LOOKUP(B58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K58" t="str">
+        <f>LOOKUP(C58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L58" t="str">
+        <f>LOOKUP(D58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M58" t="str">
+        <f>LOOKUP(E58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M90</v>
+      </c>
+      <c r="N58" t="str">
+        <f>LOOKUP(F58,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" t="s">
+        <v>78</v>
+      </c>
+      <c r="F59" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" t="s">
+        <v>61</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E14-F1-I0-</v>
+      </c>
+      <c r="I59" t="str">
+        <f>LOOKUP(A59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J59" t="str">
+        <f>LOOKUP(B59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K59" t="str">
+        <f>LOOKUP(C59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L59" t="str">
+        <f>LOOKUP(D59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M59" t="str">
+        <f>LOOKUP(E59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M90</v>
+      </c>
+      <c r="N59" t="str">
+        <f>LOOKUP(F59,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" t="s">
+        <v>61</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E15-F1-I0-</v>
+      </c>
+      <c r="I60" t="str">
+        <f>LOOKUP(A60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J60" t="str">
+        <f>LOOKUP(B60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K60" t="str">
+        <f>LOOKUP(C60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L60" t="str">
+        <f>LOOKUP(D60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M60" t="str">
+        <f>LOOKUP(E60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M110</v>
+      </c>
+      <c r="N60" t="str">
+        <f>LOOKUP(F60,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>79</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E15-F1-I0-</v>
+      </c>
+      <c r="I61" t="str">
+        <f>LOOKUP(A61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J61" t="str">
+        <f>LOOKUP(B61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K61" t="str">
+        <f>LOOKUP(C61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L61" t="str">
+        <f>LOOKUP(D61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M61" t="str">
+        <f>LOOKUP(E61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M110</v>
+      </c>
+      <c r="N61" t="str">
+        <f>LOOKUP(F61,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" t="s">
+        <v>80</v>
+      </c>
+      <c r="F62" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" t="s">
+        <v>61</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E16-F1-I0-</v>
+      </c>
+      <c r="I62" t="str">
+        <f>LOOKUP(A62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J62" t="str">
+        <f>LOOKUP(B62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K62" t="str">
+        <f>LOOKUP(C62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L62" t="str">
+        <f>LOOKUP(D62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M62" t="str">
+        <f>LOOKUP(E62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M120</v>
+      </c>
+      <c r="N62" t="str">
+        <f>LOOKUP(F62,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" t="s">
+        <v>55</v>
+      </c>
+      <c r="G63" t="s">
+        <v>61</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E16-F1-I0-</v>
+      </c>
+      <c r="I63" t="str">
+        <f>LOOKUP(A63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J63" t="str">
+        <f>LOOKUP(B63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K63" t="str">
+        <f>LOOKUP(C63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L63" t="str">
+        <f>LOOKUP(D63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M63" t="str">
+        <f>LOOKUP(E63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M120</v>
+      </c>
+      <c r="N63" t="str">
+        <f>LOOKUP(F63,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E17-F1-I0-</v>
+      </c>
+      <c r="I64" t="str">
+        <f>LOOKUP(A64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J64" t="str">
+        <f>LOOKUP(B64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K64" t="str">
+        <f>LOOKUP(C64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L64" t="str">
+        <f>LOOKUP(D64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M64" t="str">
+        <f>LOOKUP(E64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M130</v>
+      </c>
+      <c r="N64" t="str">
+        <f>LOOKUP(F64,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" t="s">
+        <v>81</v>
+      </c>
+      <c r="F65" t="s">
+        <v>55</v>
+      </c>
+      <c r="G65" t="s">
+        <v>61</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E17-F1-I0-</v>
+      </c>
+      <c r="I65" t="str">
+        <f>LOOKUP(A65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J65" t="str">
+        <f>LOOKUP(B65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K65" t="str">
+        <f>LOOKUP(C65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L65" t="str">
+        <f>LOOKUP(D65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M65" t="str">
+        <f>LOOKUP(E65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M130</v>
+      </c>
+      <c r="N65" t="str">
+        <f>LOOKUP(F65,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>82</v>
+      </c>
+      <c r="F66" t="s">
+        <v>55</v>
+      </c>
+      <c r="G66" t="s">
+        <v>61</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E18-F1-I0-</v>
+      </c>
+      <c r="I66" t="str">
+        <f>LOOKUP(A66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J66" t="str">
+        <f>LOOKUP(B66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K66" t="str">
+        <f>LOOKUP(C66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L66" t="str">
+        <f>LOOKUP(D66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M66" t="str">
+        <f>LOOKUP(E66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M140</v>
+      </c>
+      <c r="N66" t="str">
+        <f>LOOKUP(F66,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" t="s">
+        <v>55</v>
+      </c>
+      <c r="G67" t="s">
+        <v>61</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E18-F1-I0-</v>
+      </c>
+      <c r="I67" t="str">
+        <f>LOOKUP(A67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J67" t="str">
+        <f>LOOKUP(B67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K67" t="str">
+        <f>LOOKUP(C67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L67" t="str">
+        <f>LOOKUP(D67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M67" t="str">
+        <f>LOOKUP(E67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M140</v>
+      </c>
+      <c r="N67" t="str">
+        <f>LOOKUP(F67,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
+        <v>83</v>
+      </c>
+      <c r="F68" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" t="s">
+        <v>61</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D0-L10-E19-F1-I0-</v>
+      </c>
+      <c r="I68" t="str">
+        <f>LOOKUP(A68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J68" t="str">
+        <f>LOOKUP(B68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K68" t="str">
+        <f>LOOKUP(C68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L68" t="str">
+        <f>LOOKUP(D68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M68" t="str">
+        <f>LOOKUP(E68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M150</v>
+      </c>
+      <c r="N68" t="str">
+        <f>LOOKUP(F68,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" t="s">
+        <v>83</v>
+      </c>
+      <c r="F69" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" t="s">
+        <v>61</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E19-F1-I0-</v>
+      </c>
+      <c r="I69" t="str">
+        <f>LOOKUP(A69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J69" t="str">
+        <f>LOOKUP(B69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K69" t="str">
+        <f>LOOKUP(C69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L69" t="str">
+        <f>LOOKUP(D69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M69" t="str">
+        <f>LOOKUP(E69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M150</v>
+      </c>
+      <c r="N69" t="str">
+        <f>LOOKUP(F69,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:N49"/>
   <sortState ref="A2:N49">
     <sortCondition ref="F2:F49"/>
     <sortCondition ref="D2:D49"/>
@@ -3049,10 +4133,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3097,7 +4181,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C20" si="0">CONCATENATE(A3,B3)</f>
+        <f t="shared" ref="C3:C31" si="0">CONCATENATE(A3,B3)</f>
         <v>A10</v>
       </c>
       <c r="D3" t="s">
@@ -3271,91 +4355,256 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>F0</v>
+        <v>E3</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>F1</v>
+        <v>E10</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>E11</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>L10</v>
+        <v>E12</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B19">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>L30</v>
+        <v>E13</v>
       </c>
       <c r="D19" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
+        <v>E14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>E15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>E16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>17</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>E17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>E18</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>19</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>E19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>F0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>F1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>F2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>L10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>L30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31">
+        <v>31</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
         <v>L31</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D31" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix error in new missspecification files
I was estimating externally for cases that had no mla data. No two
separate set of casefiles are created and they are correctly referenced
in the spreadsheet. This did not change the number of scenarios, only
fixed scenarios that would not run.
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -12,14 +12,14 @@
     <sheet name="readme" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$69</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="105">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -304,6 +304,36 @@
   </si>
   <si>
     <t>M150</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>E22</t>
+  </si>
+  <si>
+    <t>E23</t>
+  </si>
+  <si>
+    <t>E24</t>
+  </si>
+  <si>
+    <t>E25</t>
+  </si>
+  <si>
+    <t>E26</t>
+  </si>
+  <si>
+    <t>E27</t>
+  </si>
+  <si>
+    <t>E28</t>
+  </si>
+  <si>
+    <t>E29</t>
   </si>
 </sst>
 </file>
@@ -659,8 +689,8 @@
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N63" sqref="N63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,10 +810,10 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -793,7 +823,7 @@
       </c>
       <c r="H3" t="str">
         <f>CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
-        <v>A0-C0-D0-L10-E1-F0-I0-</v>
+        <v>A0-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I3" t="str">
         <f>LOOKUP(A3,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -809,11 +839,11 @@
       </c>
       <c r="L3" t="str">
         <f>LOOKUP(D3,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M3" t="str">
         <f>LOOKUP(E3,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N3" t="str">
         <f>LOOKUP(F3,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -882,10 +912,10 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
         <v>54</v>
@@ -895,7 +925,7 @@
       </c>
       <c r="H5" t="str">
         <f>CONCATENATE(A5,"-",B5,"-",C5,"-",D5,"-",E5,"-",F5,"-",G5,"-")</f>
-        <v>A10-C0-D0-L10-E1-F0-I0-</v>
+        <v>A10-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I5" t="str">
         <f>LOOKUP(A5,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -911,11 +941,11 @@
       </c>
       <c r="L5" t="str">
         <f>LOOKUP(D5,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M5" t="str">
         <f>LOOKUP(E5,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N5" t="str">
         <f>LOOKUP(F5,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -924,19 +954,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
@@ -946,11 +976,11 @@
       </c>
       <c r="H6" t="str">
         <f>CONCATENATE(A6,"-",B6,"-",C6,"-",D6,"-",E6,"-",F6,"-",G6,"-")</f>
-        <v>A10-C0-D10-L10-E2-F0-I0-</v>
+        <v>A30-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I6" t="str">
         <f>LOOKUP(A6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J6" t="str">
         <f>LOOKUP(B6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -958,7 +988,7 @@
       </c>
       <c r="K6" t="str">
         <f>LOOKUP(C6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L6" t="str">
         <f>LOOKUP(D6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -966,7 +996,7 @@
       </c>
       <c r="M6" t="str">
         <f>LOOKUP(E6,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>fixed</v>
       </c>
       <c r="N6" t="str">
         <f>LOOKUP(F6,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -975,19 +1005,19 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
         <v>54</v>
@@ -995,26 +1025,33 @@
       <c r="G7" t="s">
         <v>61</v>
       </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" t="s">
-        <v>58</v>
+      <c r="H7" t="str">
+        <f>CONCATENATE(A7,"-",B7,"-",C7,"-",D7,"-",E7,"-",F7,"-",G7,"-")</f>
+        <v>A30-C0-D0-L30-E0-F0-I0-</v>
+      </c>
+      <c r="I7" t="str">
+        <f>LOOKUP(A7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J7" t="str">
+        <f>LOOKUP(B7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K7" t="str">
+        <f>LOOKUP(C7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L7" t="str">
+        <f>LOOKUP(D7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M7" t="str">
+        <f>LOOKUP(E7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fixed</v>
+      </c>
+      <c r="N7" t="str">
+        <f>LOOKUP(F7,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>constant</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1022,13 +1059,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -1041,7 +1078,7 @@
       </c>
       <c r="H8" t="str">
         <f>CONCATENATE(A8,"-",B8,"-",C8,"-",D8,"-",E8,"-",F8,"-",G8,"-")</f>
-        <v>A30-C0-D0-L10-E0-F0-I0-</v>
+        <v>A30-C20-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I8" t="str">
         <f>LOOKUP(A8,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1049,7 +1086,7 @@
       </c>
       <c r="J8" t="str">
         <f>LOOKUP(B8,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K8" t="str">
         <f>LOOKUP(C8,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1057,7 +1094,7 @@
       </c>
       <c r="L8" t="str">
         <f>LOOKUP(D8,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M8" t="str">
         <f>LOOKUP(E8,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1070,7 +1107,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1092,11 +1129,11 @@
       </c>
       <c r="H9" t="str">
         <f>CONCATENATE(A9,"-",B9,"-",C9,"-",D9,"-",E9,"-",F9,"-",G9,"-")</f>
-        <v>A30-C0-D0-L10-E1-F0-I0-</v>
+        <v>A0-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I9" t="str">
         <f>LOOKUP(A9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J9" t="str">
         <f>LOOKUP(B9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1121,19 +1158,19 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
@@ -1143,11 +1180,11 @@
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE(A10,"-",B10,"-",C10,"-",D10,"-",E10,"-",F10,"-",G10,"-")</f>
-        <v>A30-C0-D10-L10-E2-F0-I0-</v>
+        <v>A0-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I10" t="str">
         <f>LOOKUP(A10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J10" t="str">
         <f>LOOKUP(B10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1155,15 +1192,15 @@
       </c>
       <c r="K10" t="str">
         <f>LOOKUP(C10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L10" t="str">
         <f>LOOKUP(D10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M10" t="str">
         <f>LOOKUP(E10,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N10" t="str">
         <f>LOOKUP(F10,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1172,19 +1209,19 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
@@ -1192,31 +1229,38 @@
       <c r="G11" t="s">
         <v>61</v>
       </c>
-      <c r="H11" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" t="s">
-        <v>58</v>
+      <c r="H11" t="str">
+        <f>CONCATENATE(A11,"-",B11,"-",C11,"-",D11,"-",E11,"-",F11,"-",G11,"-")</f>
+        <v>A10-C0-D0-L10-E1-F0-I0-</v>
+      </c>
+      <c r="I11" t="str">
+        <f>LOOKUP(A11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J11" t="str">
+        <f>LOOKUP(B11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K11" t="str">
+        <f>LOOKUP(C11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L11" t="str">
+        <f>LOOKUP(D11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M11" t="str">
+        <f>LOOKUP(E11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>internal</v>
+      </c>
+      <c r="N11" t="str">
+        <f>LOOKUP(F11,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>constant</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -1228,7 +1272,7 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
@@ -1238,11 +1282,11 @@
       </c>
       <c r="H12" t="str">
         <f>CONCATENATE(A12,"-",B12,"-",C12,"-",D12,"-",E12,"-",F12,"-",G12,"-")</f>
-        <v>A0-C0-D0-L30-E0-F0-I0-</v>
+        <v>A10-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I12" t="str">
         <f>LOOKUP(A12,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish age</v>
       </c>
       <c r="J12" t="str">
         <f>LOOKUP(B12,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1258,7 +1302,7 @@
       </c>
       <c r="M12" t="str">
         <f>LOOKUP(E12,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N12" t="str">
         <f>LOOKUP(F12,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1267,7 +1311,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -1276,7 +1320,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>19</v>
@@ -1289,11 +1333,11 @@
       </c>
       <c r="H13" t="str">
         <f>CONCATENATE(A13,"-",B13,"-",C13,"-",D13,"-",E13,"-",F13,"-",G13,"-")</f>
-        <v>A0-C0-D0-L30-E1-F0-I0-</v>
+        <v>A30-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I13" t="str">
         <f>LOOKUP(A13,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J13" t="str">
         <f>LOOKUP(B13,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1305,7 +1349,7 @@
       </c>
       <c r="L13" t="str">
         <f>LOOKUP(D13,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M13" t="str">
         <f>LOOKUP(E13,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1318,7 +1362,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
@@ -1330,7 +1374,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
@@ -1340,11 +1384,11 @@
       </c>
       <c r="H14" t="str">
         <f>CONCATENATE(A14,"-",B14,"-",C14,"-",D14,"-",E14,"-",F14,"-",G14,"-")</f>
-        <v>A10-C0-D0-L30-E0-F0-I0-</v>
+        <v>A30-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I14" t="str">
         <f>LOOKUP(A14,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J14" t="str">
         <f>LOOKUP(B14,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1360,7 +1404,7 @@
       </c>
       <c r="M14" t="str">
         <f>LOOKUP(E14,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N14" t="str">
         <f>LOOKUP(F14,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1369,10 +1413,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1391,15 +1435,15 @@
       </c>
       <c r="H15" t="str">
         <f>CONCATENATE(A15,"-",B15,"-",C15,"-",D15,"-",E15,"-",F15,"-",G15,"-")</f>
-        <v>A10-C0-D0-L30-E1-F0-I0-</v>
+        <v>A30-C20-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I15" t="str">
         <f>LOOKUP(A15,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J15" t="str">
         <f>LOOKUP(B15,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K15" t="str">
         <f>LOOKUP(C15,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1429,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -1442,7 +1486,7 @@
       </c>
       <c r="H16" t="str">
         <f>CONCATENATE(A16,"-",B16,"-",C16,"-",D16,"-",E16,"-",F16,"-",G16,"-")</f>
-        <v>A10-C0-D10-L30-E2-F0-I0-</v>
+        <v>A10-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I16" t="str">
         <f>LOOKUP(A16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1458,7 +1502,7 @@
       </c>
       <c r="L16" t="str">
         <f>LOOKUP(D16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M16" t="str">
         <f>LOOKUP(E16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1483,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
         <v>54</v>
@@ -1491,26 +1535,33 @@
       <c r="G17" t="s">
         <v>61</v>
       </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" t="s">
-        <v>48</v>
-      </c>
-      <c r="N17" t="s">
-        <v>58</v>
+      <c r="H17" t="str">
+        <f>CONCATENATE(A17,"-",B17,"-",C17,"-",D17,"-",E17,"-",F17,"-",G17,"-")</f>
+        <v>A10-C0-D10-L30-E2-F0-I0-</v>
+      </c>
+      <c r="I17" t="str">
+        <f>LOOKUP(A17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J17" t="str">
+        <f>LOOKUP(B17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K17" t="str">
+        <f>LOOKUP(C17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L17" t="str">
+        <f>LOOKUP(D17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M17" t="str">
+        <f>LOOKUP(E17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M150</v>
+      </c>
+      <c r="N17" t="str">
+        <f>LOOKUP(F17,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>constant</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1521,13 +1572,13 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
         <v>54</v>
@@ -1537,7 +1588,7 @@
       </c>
       <c r="H18" t="str">
         <f>CONCATENATE(A18,"-",B18,"-",C18,"-",D18,"-",E18,"-",F18,"-",G18,"-")</f>
-        <v>A30-C0-D0-L30-E0-F0-I0-</v>
+        <v>A30-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I18" t="str">
         <f>LOOKUP(A18,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1549,15 +1600,15 @@
       </c>
       <c r="K18" t="str">
         <f>LOOKUP(C18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L18" t="str">
         <f>LOOKUP(D18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M18" t="str">
         <f>LOOKUP(E18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M150</v>
       </c>
       <c r="N18" t="str">
         <f>LOOKUP(F18,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1572,13 +1623,13 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
         <v>54</v>
@@ -1588,7 +1639,7 @@
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE(A19,"-",B19,"-",C19,"-",D19,"-",E19,"-",F19,"-",G19,"-")</f>
-        <v>A30-C0-D0-L30-E1-F0-I0-</v>
+        <v>A30-C0-D10-L30-E2-F0-I0-</v>
       </c>
       <c r="I19" t="str">
         <f>LOOKUP(A19,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1600,7 +1651,7 @@
       </c>
       <c r="K19" t="str">
         <f>LOOKUP(C19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L19" t="str">
         <f>LOOKUP(D19,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1608,7 +1659,7 @@
       </c>
       <c r="M19" t="str">
         <f>LOOKUP(E19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M150</v>
       </c>
       <c r="N19" t="str">
         <f>LOOKUP(F19,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1620,16 +1671,16 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
         <v>54</v>
@@ -1639,7 +1690,7 @@
       </c>
       <c r="H20" t="str">
         <f>CONCATENATE(A20,"-",B20,"-",C20,"-",D20,"-",E20,"-",F20,"-",G20,"-")</f>
-        <v>A30-C20-D0-L30-E0-F0-I0-</v>
+        <v>A30-C0-D20-L30-E2-F0-I0-</v>
       </c>
       <c r="I20" t="str">
         <f>LOOKUP(A20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1647,11 +1698,11 @@
       </c>
       <c r="J20" t="str">
         <f>LOOKUP(B20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K20" t="str">
         <f>LOOKUP(C20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>surv mlacomp</v>
       </c>
       <c r="L20" t="str">
         <f>LOOKUP(D20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1659,7 +1710,7 @@
       </c>
       <c r="M20" t="str">
         <f>LOOKUP(E20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M150</v>
       </c>
       <c r="N20" t="str">
         <f>LOOKUP(F20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1668,19 +1719,19 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
         <v>54</v>
@@ -1688,38 +1739,31 @@
       <c r="G21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" t="str">
-        <f>CONCATENATE(A21,"-",B21,"-",C21,"-",D21,"-",E21,"-",F21,"-",G21,"-")</f>
-        <v>A30-C20-D0-L30-E1-F0-I0-</v>
-      </c>
-      <c r="I21" t="str">
-        <f>LOOKUP(A21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J21" t="str">
-        <f>LOOKUP(B21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
-      </c>
-      <c r="K21" t="str">
-        <f>LOOKUP(C21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L21" t="str">
-        <f>LOOKUP(D21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M21" t="str">
-        <f>LOOKUP(E21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
-      </c>
-      <c r="N21" t="str">
-        <f>LOOKUP(F21,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
@@ -1731,7 +1775,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -1739,33 +1783,26 @@
       <c r="G22" t="s">
         <v>61</v>
       </c>
-      <c r="H22" t="str">
-        <f>CONCATENATE(A22,"-",B22,"-",C22,"-",D22,"-",E22,"-",F22,"-",G22,"-")</f>
-        <v>A30-C0-D10-L30-E2-F0-I0-</v>
-      </c>
-      <c r="I22" t="str">
-        <f>LOOKUP(A22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J22" t="str">
-        <f>LOOKUP(B22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K22" t="str">
-        <f>LOOKUP(C22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
-      </c>
-      <c r="L22" t="str">
-        <f>LOOKUP(D22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M22" t="str">
-        <f>LOOKUP(E22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
-      </c>
-      <c r="N22" t="str">
-        <f>LOOKUP(F22,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1779,7 +1816,7 @@
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>73</v>
@@ -1791,7 +1828,7 @@
         <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I23" t="s">
         <v>0</v>
@@ -1803,7 +1840,7 @@
         <v>14</v>
       </c>
       <c r="L23" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M23" t="s">
         <v>48</v>
@@ -1820,13 +1857,13 @@
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="F24" t="s">
         <v>54</v>
@@ -1834,33 +1871,26 @@
       <c r="G24" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="str">
-        <f>CONCATENATE(A24,"-",B24,"-",C24,"-",D24,"-",E24,"-",F24,"-",G24,"-")</f>
-        <v>A30-C0-D20-L30-E2-F0-I0-</v>
-      </c>
-      <c r="I24" t="str">
-        <f>LOOKUP(A24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="J24" t="str">
-        <f>LOOKUP(B24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K24" t="str">
-        <f>LOOKUP(C24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv mlacomp</v>
-      </c>
-      <c r="L24" t="str">
-        <f>LOOKUP(D24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
-      </c>
-      <c r="M24" t="str">
-        <f>LOOKUP(E24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
-      </c>
-      <c r="N24" t="str">
-        <f>LOOKUP(F24,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>constant</v>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>48</v>
+      </c>
+      <c r="N24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1969,10 +1999,10 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F27" t="s">
         <v>55</v>
@@ -1982,7 +2012,7 @@
       </c>
       <c r="H27" t="str">
         <f>CONCATENATE(A27,"-",B27,"-",C27,"-",D27,"-",E27,"-",F27,"-",G27,"-")</f>
-        <v>A0-C0-D0-L10-E1-F1-I0-</v>
+        <v>A0-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I27" t="str">
         <f>LOOKUP(A27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1998,11 +2028,11 @@
       </c>
       <c r="L27" t="str">
         <f>LOOKUP(D27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M27" t="str">
         <f>LOOKUP(E27,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N27" t="str">
         <f>LOOKUP(F27,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2071,10 +2101,10 @@
         <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
         <v>55</v>
@@ -2084,7 +2114,7 @@
       </c>
       <c r="H29" t="str">
         <f>CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
-        <v>A10-C0-D0-L10-E1-F1-I0-</v>
+        <v>A10-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I29" t="str">
         <f>LOOKUP(A29,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2100,11 +2130,11 @@
       </c>
       <c r="L29" t="str">
         <f>LOOKUP(D29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M29" t="str">
         <f>LOOKUP(E29,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>fixed</v>
       </c>
       <c r="N29" t="str">
         <f>LOOKUP(F29,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2113,19 +2143,19 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
         <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F30" t="s">
         <v>55</v>
@@ -2135,11 +2165,11 @@
       </c>
       <c r="H30" t="str">
         <f>CONCATENATE(A30,"-",B30,"-",C30,"-",D30,"-",E30,"-",F30,"-",G30,"-")</f>
-        <v>A10-C0-D10-L10-E2-F1-I0-</v>
+        <v>A30-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I30" t="str">
         <f>LOOKUP(A30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J30" t="str">
         <f>LOOKUP(B30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2147,7 +2177,7 @@
       </c>
       <c r="K30" t="str">
         <f>LOOKUP(C30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L30" t="str">
         <f>LOOKUP(D30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2155,7 +2185,7 @@
       </c>
       <c r="M30" t="str">
         <f>LOOKUP(E30,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>fixed</v>
       </c>
       <c r="N30" t="str">
         <f>LOOKUP(F30,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2164,19 +2194,19 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="F31" t="s">
         <v>55</v>
@@ -2184,26 +2214,33 @@
       <c r="G31" t="s">
         <v>61</v>
       </c>
-      <c r="H31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" t="s">
-        <v>16</v>
-      </c>
-      <c r="M31" t="s">
-        <v>48</v>
-      </c>
-      <c r="N31" t="s">
-        <v>59</v>
+      <c r="H31" t="str">
+        <f>CONCATENATE(A31,"-",B31,"-",C31,"-",D31,"-",E31,"-",F31,"-",G31,"-")</f>
+        <v>A30-C0-D0-L30-E0-F1-I0-</v>
+      </c>
+      <c r="I31" t="str">
+        <f>LOOKUP(A31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="J31" t="str">
+        <f>LOOKUP(B31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K31" t="str">
+        <f>LOOKUP(C31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L31" t="str">
+        <f>LOOKUP(D31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish &amp; surv length</v>
+      </c>
+      <c r="M31" t="str">
+        <f>LOOKUP(E31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fixed</v>
+      </c>
+      <c r="N31" t="str">
+        <f>LOOKUP(F31,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -2211,13 +2248,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
         <v>23</v>
@@ -2230,7 +2267,7 @@
       </c>
       <c r="H32" t="str">
         <f>CONCATENATE(A32,"-",B32,"-",C32,"-",D32,"-",E32,"-",F32,"-",G32,"-")</f>
-        <v>A30-C0-D0-L10-E0-F1-I0-</v>
+        <v>A30-C20-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I32" t="str">
         <f>LOOKUP(A32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2238,7 +2275,7 @@
       </c>
       <c r="J32" t="str">
         <f>LOOKUP(B32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K32" t="str">
         <f>LOOKUP(C32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2246,7 +2283,7 @@
       </c>
       <c r="L32" t="str">
         <f>LOOKUP(D32,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M32" t="str">
         <f>LOOKUP(E32,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2259,7 +2296,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
         <v>13</v>
@@ -2281,11 +2318,11 @@
       </c>
       <c r="H33" t="str">
         <f>CONCATENATE(A33,"-",B33,"-",C33,"-",D33,"-",E33,"-",F33,"-",G33,"-")</f>
-        <v>A30-C0-D0-L10-E1-F1-I0-</v>
+        <v>A0-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I33" t="str">
         <f>LOOKUP(A33,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J33" t="str">
         <f>LOOKUP(B33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2310,19 +2347,19 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F34" t="s">
         <v>55</v>
@@ -2332,11 +2369,11 @@
       </c>
       <c r="H34" t="str">
         <f>CONCATENATE(A34,"-",B34,"-",C34,"-",D34,"-",E34,"-",F34,"-",G34,"-")</f>
-        <v>A30-C0-D10-L10-E2-F1-I0-</v>
+        <v>A0-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I34" t="str">
         <f>LOOKUP(A34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>no age</v>
       </c>
       <c r="J34" t="str">
         <f>LOOKUP(B34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2344,15 +2381,15 @@
       </c>
       <c r="K34" t="str">
         <f>LOOKUP(C34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L34" t="str">
         <f>LOOKUP(D34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M34" t="str">
         <f>LOOKUP(E34,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N34" t="str">
         <f>LOOKUP(F34,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2361,19 +2398,19 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F35" t="s">
         <v>55</v>
@@ -2381,31 +2418,38 @@
       <c r="G35" t="s">
         <v>61</v>
       </c>
-      <c r="H35" t="s">
-        <v>68</v>
-      </c>
-      <c r="I35" t="s">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" t="s">
-        <v>48</v>
-      </c>
-      <c r="N35" t="s">
-        <v>59</v>
+      <c r="H35" t="str">
+        <f>CONCATENATE(A35,"-",B35,"-",C35,"-",D35,"-",E35,"-",F35,"-",G35,"-")</f>
+        <v>A10-C0-D0-L10-E1-F1-I0-</v>
+      </c>
+      <c r="I35" t="str">
+        <f>LOOKUP(A35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J35" t="str">
+        <f>LOOKUP(B35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K35" t="str">
+        <f>LOOKUP(C35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no mlacomp</v>
+      </c>
+      <c r="L35" t="str">
+        <f>LOOKUP(D35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M35" t="str">
+        <f>LOOKUP(E35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>internal</v>
+      </c>
+      <c r="N35" t="str">
+        <f>LOOKUP(F35,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
         <v>13</v>
@@ -2417,7 +2461,7 @@
         <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F36" t="s">
         <v>55</v>
@@ -2427,11 +2471,11 @@
       </c>
       <c r="H36" t="str">
         <f>CONCATENATE(A36,"-",B36,"-",C36,"-",D36,"-",E36,"-",F36,"-",G36,"-")</f>
-        <v>A0-C0-D0-L30-E0-F1-I0-</v>
+        <v>A10-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I36" t="str">
         <f>LOOKUP(A36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish age</v>
       </c>
       <c r="J36" t="str">
         <f>LOOKUP(B36,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2447,7 +2491,7 @@
       </c>
       <c r="M36" t="str">
         <f>LOOKUP(E36,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N36" t="str">
         <f>LOOKUP(F36,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2456,7 +2500,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
         <v>13</v>
@@ -2465,7 +2509,7 @@
         <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -2478,11 +2522,11 @@
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE(A37,"-",B37,"-",C37,"-",D37,"-",E37,"-",F37,"-",G37,"-")</f>
-        <v>A0-C0-D0-L30-E1-F1-I0-</v>
+        <v>A30-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I37" t="str">
         <f>LOOKUP(A37,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J37" t="str">
         <f>LOOKUP(B37,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2494,7 +2538,7 @@
       </c>
       <c r="L37" t="str">
         <f>LOOKUP(D37,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M37" t="str">
         <f>LOOKUP(E37,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2507,7 +2551,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
@@ -2519,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F38" t="s">
         <v>55</v>
@@ -2529,11 +2573,11 @@
       </c>
       <c r="H38" t="str">
         <f>CONCATENATE(A38,"-",B38,"-",C38,"-",D38,"-",E38,"-",F38,"-",G38,"-")</f>
-        <v>A10-C0-D0-L30-E0-F1-I0-</v>
+        <v>A30-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I38" t="str">
         <f>LOOKUP(A38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J38" t="str">
         <f>LOOKUP(B38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2549,7 +2593,7 @@
       </c>
       <c r="M38" t="str">
         <f>LOOKUP(E38,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>internal</v>
       </c>
       <c r="N38" t="str">
         <f>LOOKUP(F38,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2558,10 +2602,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
         <v>20</v>
@@ -2580,15 +2624,15 @@
       </c>
       <c r="H39" t="str">
         <f>CONCATENATE(A39,"-",B39,"-",C39,"-",D39,"-",E39,"-",F39,"-",G39,"-")</f>
-        <v>A10-C0-D0-L30-E1-F1-I0-</v>
+        <v>A30-C20-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I39" t="str">
         <f>LOOKUP(A39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J39" t="str">
         <f>LOOKUP(B39,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
+        <v>surv calcomp</v>
       </c>
       <c r="K39" t="str">
         <f>LOOKUP(C39,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2618,10 +2662,10 @@
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F40" t="s">
         <v>55</v>
@@ -2631,7 +2675,7 @@
       </c>
       <c r="H40" t="str">
         <f>CONCATENATE(A40,"-",B40,"-",C40,"-",D40,"-",E40,"-",F40,"-",G40,"-")</f>
-        <v>A10-C0-D10-L30-E2-F1-I0-</v>
+        <v>A10-C0-D10-L10-E10-F1-I0-</v>
       </c>
       <c r="I40" t="str">
         <f>LOOKUP(A40,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2647,11 +2691,11 @@
       </c>
       <c r="L40" t="str">
         <f>LOOKUP(D40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M40" t="str">
         <f>LOOKUP(E40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>M50</v>
       </c>
       <c r="N40" t="str">
         <f>LOOKUP(F40,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2669,10 +2713,10 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F41" t="s">
         <v>55</v>
@@ -2680,43 +2724,50 @@
       <c r="G41" t="s">
         <v>61</v>
       </c>
-      <c r="H41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41" t="s">
-        <v>12</v>
-      </c>
-      <c r="K41" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M41" t="s">
-        <v>48</v>
-      </c>
-      <c r="N41" t="s">
-        <v>59</v>
+      <c r="H41" t="str">
+        <f>CONCATENATE(A41,"-",B41,"-",C41,"-",D41,"-",E41,"-",F41,"-",G41,"-")</f>
+        <v>A10-C0-D10-L10-E11-F1-I0-</v>
+      </c>
+      <c r="I41" t="str">
+        <f>LOOKUP(A41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J41" t="str">
+        <f>LOOKUP(B41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K41" t="str">
+        <f>LOOKUP(C41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L41" t="str">
+        <f>LOOKUP(D41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M41" t="str">
+        <f>LOOKUP(E41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M60</v>
+      </c>
+      <c r="N41" t="str">
+        <f>LOOKUP(F41,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
         <v>55</v>
@@ -2726,11 +2777,11 @@
       </c>
       <c r="H42" t="str">
         <f>CONCATENATE(A42,"-",B42,"-",C42,"-",D42,"-",E42,"-",F42,"-",G42,"-")</f>
-        <v>A30-C0-D0-L30-E0-F1-I0-</v>
+        <v>A10-C0-D10-L10-E12-F1-I0-</v>
       </c>
       <c r="I42" t="str">
         <f>LOOKUP(A42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J42" t="str">
         <f>LOOKUP(B42,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2738,15 +2789,15 @@
       </c>
       <c r="K42" t="str">
         <f>LOOKUP(C42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L42" t="str">
         <f>LOOKUP(D42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M42" t="str">
         <f>LOOKUP(E42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M70</v>
       </c>
       <c r="N42" t="str">
         <f>LOOKUP(F42,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2755,19 +2806,19 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="F43" t="s">
         <v>55</v>
@@ -2777,11 +2828,11 @@
       </c>
       <c r="H43" t="str">
         <f>CONCATENATE(A43,"-",B43,"-",C43,"-",D43,"-",E43,"-",F43,"-",G43,"-")</f>
-        <v>A30-C0-D0-L30-E1-F1-I0-</v>
+        <v>A10-C0-D10-L10-E13-F1-I0-</v>
       </c>
       <c r="I43" t="str">
         <f>LOOKUP(A43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J43" t="str">
         <f>LOOKUP(B43,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2789,15 +2840,15 @@
       </c>
       <c r="K43" t="str">
         <f>LOOKUP(C43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L43" t="str">
         <f>LOOKUP(D43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M43" t="str">
         <f>LOOKUP(E43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M80</v>
       </c>
       <c r="N43" t="str">
         <f>LOOKUP(F43,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2806,19 +2857,19 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="F44" t="s">
         <v>55</v>
@@ -2828,27 +2879,27 @@
       </c>
       <c r="H44" t="str">
         <f>CONCATENATE(A44,"-",B44,"-",C44,"-",D44,"-",E44,"-",F44,"-",G44,"-")</f>
-        <v>A30-C20-D0-L30-E0-F1-I0-</v>
+        <v>A10-C0-D10-L10-E14-F1-I0-</v>
       </c>
       <c r="I44" t="str">
         <f>LOOKUP(A44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J44" t="str">
         <f>LOOKUP(B44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K44" t="str">
         <f>LOOKUP(C44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L44" t="str">
         <f>LOOKUP(D44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M44" t="str">
         <f>LOOKUP(E44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M90</v>
       </c>
       <c r="N44" t="str">
         <f>LOOKUP(F44,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2857,19 +2908,19 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F45" t="s">
         <v>55</v>
@@ -2879,27 +2930,27 @@
       </c>
       <c r="H45" t="str">
         <f>CONCATENATE(A45,"-",B45,"-",C45,"-",D45,"-",E45,"-",F45,"-",G45,"-")</f>
-        <v>A30-C20-D0-L30-E1-F1-I0-</v>
+        <v>A10-C0-D10-L10-E15-F1-I0-</v>
       </c>
       <c r="I45" t="str">
         <f>LOOKUP(A45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J45" t="str">
         <f>LOOKUP(B45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv calcomp</v>
+        <v>no calcomp</v>
       </c>
       <c r="K45" t="str">
         <f>LOOKUP(C45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L45" t="str">
         <f>LOOKUP(D45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M45" t="str">
         <f>LOOKUP(E45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M110</v>
       </c>
       <c r="N45" t="str">
         <f>LOOKUP(F45,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2908,7 +2959,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -2917,10 +2968,10 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="F46" t="s">
         <v>55</v>
@@ -2930,11 +2981,11 @@
       </c>
       <c r="H46" t="str">
         <f>CONCATENATE(A46,"-",B46,"-",C46,"-",D46,"-",E46,"-",F46,"-",G46,"-")</f>
-        <v>A30-C0-D10-L30-E2-F1-I0-</v>
+        <v>A10-C0-D10-L10-E16-F1-I0-</v>
       </c>
       <c r="I46" t="str">
         <f>LOOKUP(A46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J46" t="str">
         <f>LOOKUP(B46,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2946,11 +2997,11 @@
       </c>
       <c r="L46" t="str">
         <f>LOOKUP(D46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M46" t="str">
         <f>LOOKUP(E46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>M120</v>
       </c>
       <c r="N46" t="str">
         <f>LOOKUP(F46,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2959,7 +3010,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -2968,10 +3019,10 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F47" t="s">
         <v>55</v>
@@ -2979,43 +3030,50 @@
       <c r="G47" t="s">
         <v>61</v>
       </c>
-      <c r="H47" t="s">
-        <v>71</v>
-      </c>
-      <c r="I47" t="s">
-        <v>0</v>
-      </c>
-      <c r="J47" t="s">
-        <v>12</v>
-      </c>
-      <c r="K47" t="s">
-        <v>14</v>
-      </c>
-      <c r="L47" t="s">
-        <v>0</v>
-      </c>
-      <c r="M47" t="s">
-        <v>48</v>
-      </c>
-      <c r="N47" t="s">
-        <v>59</v>
+      <c r="H47" t="str">
+        <f>CONCATENATE(A47,"-",B47,"-",C47,"-",D47,"-",E47,"-",F47,"-",G47,"-")</f>
+        <v>A10-C0-D10-L10-E17-F1-I0-</v>
+      </c>
+      <c r="I47" t="str">
+        <f>LOOKUP(A47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J47" t="str">
+        <f>LOOKUP(B47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K47" t="str">
+        <f>LOOKUP(C47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L47" t="str">
+        <f>LOOKUP(D47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M47" t="str">
+        <f>LOOKUP(E47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M130</v>
+      </c>
+      <c r="N47" t="str">
+        <f>LOOKUP(F47,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="F48" t="s">
         <v>55</v>
@@ -3025,11 +3083,11 @@
       </c>
       <c r="H48" t="str">
         <f>CONCATENATE(A48,"-",B48,"-",C48,"-",D48,"-",E48,"-",F48,"-",G48,"-")</f>
-        <v>A30-C0-D20-L30-E2-F1-I0-</v>
+        <v>A10-C0-D10-L10-E18-F1-I0-</v>
       </c>
       <c r="I48" t="str">
         <f>LOOKUP(A48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish age</v>
       </c>
       <c r="J48" t="str">
         <f>LOOKUP(B48,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3037,15 +3095,15 @@
       </c>
       <c r="K48" t="str">
         <f>LOOKUP(C48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>surv mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L48" t="str">
         <f>LOOKUP(D48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish &amp; surv length</v>
+        <v>fish length</v>
       </c>
       <c r="M48" t="str">
         <f>LOOKUP(E48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>M140</v>
       </c>
       <c r="N48" t="str">
         <f>LOOKUP(F48,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3054,19 +3112,19 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F49" t="s">
         <v>55</v>
@@ -3074,26 +3132,33 @@
       <c r="G49" t="s">
         <v>61</v>
       </c>
-      <c r="H49" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" t="s">
-        <v>0</v>
-      </c>
-      <c r="J49" t="s">
-        <v>12</v>
-      </c>
-      <c r="K49" t="s">
-        <v>1</v>
-      </c>
-      <c r="L49" t="s">
-        <v>0</v>
-      </c>
-      <c r="M49" t="s">
-        <v>48</v>
-      </c>
-      <c r="N49" t="s">
-        <v>59</v>
+      <c r="H49" t="str">
+        <f>CONCATENATE(A49,"-",B49,"-",C49,"-",D49,"-",E49,"-",F49,"-",G49,"-")</f>
+        <v>A10-C0-D10-L10-E19-F1-I0-</v>
+      </c>
+      <c r="I49" t="str">
+        <f>LOOKUP(A49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish age</v>
+      </c>
+      <c r="J49" t="str">
+        <f>LOOKUP(B49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>no calcomp</v>
+      </c>
+      <c r="K49" t="str">
+        <f>LOOKUP(C49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish mlacomp</v>
+      </c>
+      <c r="L49" t="str">
+        <f>LOOKUP(D49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>fish length</v>
+      </c>
+      <c r="M49" t="str">
+        <f>LOOKUP(E49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>M150</v>
+      </c>
+      <c r="N49" t="str">
+        <f>LOOKUP(F49,descriptions!$C:$C,descriptions!$D:$D)</f>
+        <v>contrast</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -3104,13 +3169,13 @@
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D50" t="s">
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F50" t="s">
         <v>55</v>
@@ -3120,7 +3185,7 @@
       </c>
       <c r="H50" t="str">
         <f>CONCATENATE(A50,"-",B50,"-",C50,"-",D50,"-",E50,"-",F50,"-",G50,"-")</f>
-        <v>A10-C0-D0-L10-E10-F1-I0-</v>
+        <v>A10-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I50" t="str">
         <f>LOOKUP(A50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3132,7 +3197,7 @@
       </c>
       <c r="K50" t="str">
         <f>LOOKUP(C50,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L50" t="str">
         <f>LOOKUP(D50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3140,7 +3205,7 @@
       </c>
       <c r="M50" t="str">
         <f>LOOKUP(E50,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>M150</v>
       </c>
       <c r="N50" t="str">
         <f>LOOKUP(F50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3158,10 +3223,10 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
@@ -3171,7 +3236,7 @@
       </c>
       <c r="H51" t="str">
         <f>CONCATENATE(A51,"-",B51,"-",C51,"-",D51,"-",E51,"-",F51,"-",G51,"-")</f>
-        <v>A10-C0-D10-L10-E10-F1-I0-</v>
+        <v>A10-C0-D10-L30-E2-F1-I0-</v>
       </c>
       <c r="I51" t="str">
         <f>LOOKUP(A51,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3187,11 +3252,11 @@
       </c>
       <c r="L51" t="str">
         <f>LOOKUP(D51,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M51" t="str">
         <f>LOOKUP(E51,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>M150</v>
       </c>
       <c r="N51" t="str">
         <f>LOOKUP(F51,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3200,19 +3265,19 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
       </c>
       <c r="E52" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="F52" t="s">
         <v>55</v>
@@ -3222,11 +3287,11 @@
       </c>
       <c r="H52" t="str">
         <f>CONCATENATE(A52,"-",B52,"-",C52,"-",D52,"-",E52,"-",F52,"-",G52,"-")</f>
-        <v>A10-C0-D0-L10-E11-F1-I0-</v>
+        <v>A30-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I52" t="str">
         <f>LOOKUP(A52,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J52" t="str">
         <f>LOOKUP(B52,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3234,7 +3299,7 @@
       </c>
       <c r="K52" t="str">
         <f>LOOKUP(C52,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>fish mlacomp</v>
       </c>
       <c r="L52" t="str">
         <f>LOOKUP(D52,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3242,7 +3307,7 @@
       </c>
       <c r="M52" t="str">
         <f>LOOKUP(E52,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M60</v>
+        <v>M150</v>
       </c>
       <c r="N52" t="str">
         <f>LOOKUP(F52,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3251,7 +3316,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
         <v>13</v>
@@ -3260,10 +3325,10 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="F53" t="s">
         <v>55</v>
@@ -3273,11 +3338,11 @@
       </c>
       <c r="H53" t="str">
         <f>CONCATENATE(A53,"-",B53,"-",C53,"-",D53,"-",E53,"-",F53,"-",G53,"-")</f>
-        <v>A10-C0-D10-L10-E11-F1-I0-</v>
+        <v>A30-C0-D10-L30-E2-F1-I0-</v>
       </c>
       <c r="I53" t="str">
         <f>LOOKUP(A53,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J53" t="str">
         <f>LOOKUP(B53,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3289,11 +3354,11 @@
       </c>
       <c r="L53" t="str">
         <f>LOOKUP(D53,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M53" t="str">
         <f>LOOKUP(E53,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M60</v>
+        <v>M150</v>
       </c>
       <c r="N53" t="str">
         <f>LOOKUP(F53,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3302,19 +3367,19 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="F54" t="s">
         <v>55</v>
@@ -3323,12 +3388,12 @@
         <v>61</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" ref="H54:H69" si="0">CONCATENATE(A54,"-",B54,"-",C54,"-",D54,"-",E54,"-",F54,"-",G54,"-")</f>
-        <v>A10-C0-D0-L10-E12-F1-I0-</v>
+        <f>CONCATENATE(A54,"-",B54,"-",C54,"-",D54,"-",E54,"-",F54,"-",G54,"-")</f>
+        <v>A30-C0-D20-L30-E2-F1-I0-</v>
       </c>
       <c r="I54" t="str">
         <f>LOOKUP(A54,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J54" t="str">
         <f>LOOKUP(B54,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3336,15 +3401,15 @@
       </c>
       <c r="K54" t="str">
         <f>LOOKUP(C54,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
+        <v>surv mlacomp</v>
       </c>
       <c r="L54" t="str">
         <f>LOOKUP(D54,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M54" t="str">
         <f>LOOKUP(E54,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M70</v>
+        <v>M150</v>
       </c>
       <c r="N54" t="str">
         <f>LOOKUP(F54,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3359,13 +3424,13 @@
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -3374,8 +3439,8 @@
         <v>61</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E12-F1-I0-</v>
+        <f>CONCATENATE(A55,"-",B55,"-",C55,"-",D55,"-",E55,"-",F55,"-",G55,"-")</f>
+        <v>A10-C0-D0-L10-E20-F1-I0-</v>
       </c>
       <c r="I55" t="str">
         <f>LOOKUP(A55,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3387,7 +3452,7 @@
       </c>
       <c r="K55" t="str">
         <f>LOOKUP(C55,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L55" t="str">
         <f>LOOKUP(D55,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3395,7 +3460,7 @@
       </c>
       <c r="M55" t="str">
         <f>LOOKUP(E55,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M70</v>
+        <v>M150</v>
       </c>
       <c r="N55" t="str">
         <f>LOOKUP(F55,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3416,7 +3481,7 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
@@ -3425,8 +3490,8 @@
         <v>61</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E13-F1-I0-</v>
+        <f>CONCATENATE(A56,"-",B56,"-",C56,"-",D56,"-",E56,"-",F56,"-",G56,"-")</f>
+        <v>A10-C0-D0-L10-E21-F1-I0-</v>
       </c>
       <c r="I56" t="str">
         <f>LOOKUP(A56,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3446,7 +3511,7 @@
       </c>
       <c r="M56" t="str">
         <f>LOOKUP(E56,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M80</v>
+        <v>M150</v>
       </c>
       <c r="N56" t="str">
         <f>LOOKUP(F56,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3461,13 +3526,13 @@
         <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
@@ -3476,8 +3541,8 @@
         <v>61</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E13-F1-I0-</v>
+        <f>CONCATENATE(A57,"-",B57,"-",C57,"-",D57,"-",E57,"-",F57,"-",G57,"-")</f>
+        <v>A10-C0-D0-L10-E22-F1-I0-</v>
       </c>
       <c r="I57" t="str">
         <f>LOOKUP(A57,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3489,7 +3554,7 @@
       </c>
       <c r="K57" t="str">
         <f>LOOKUP(C57,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L57" t="str">
         <f>LOOKUP(D57,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3497,7 +3562,7 @@
       </c>
       <c r="M57" t="str">
         <f>LOOKUP(E57,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M80</v>
+        <v>M150</v>
       </c>
       <c r="N57" t="str">
         <f>LOOKUP(F57,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3518,7 +3583,7 @@
         <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
@@ -3527,8 +3592,8 @@
         <v>61</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E14-F1-I0-</v>
+        <f>CONCATENATE(A58,"-",B58,"-",C58,"-",D58,"-",E58,"-",F58,"-",G58,"-")</f>
+        <v>A10-C0-D0-L10-E23-F1-I0-</v>
       </c>
       <c r="I58" t="str">
         <f>LOOKUP(A58,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3548,7 +3613,7 @@
       </c>
       <c r="M58" t="str">
         <f>LOOKUP(E58,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M90</v>
+        <v>M150</v>
       </c>
       <c r="N58" t="str">
         <f>LOOKUP(F58,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3563,13 +3628,13 @@
         <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
@@ -3578,8 +3643,8 @@
         <v>61</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E14-F1-I0-</v>
+        <f>CONCATENATE(A59,"-",B59,"-",C59,"-",D59,"-",E59,"-",F59,"-",G59,"-")</f>
+        <v>A10-C0-D0-L10-E24-F1-I0-</v>
       </c>
       <c r="I59" t="str">
         <f>LOOKUP(A59,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3591,7 +3656,7 @@
       </c>
       <c r="K59" t="str">
         <f>LOOKUP(C59,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L59" t="str">
         <f>LOOKUP(D59,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3599,7 +3664,7 @@
       </c>
       <c r="M59" t="str">
         <f>LOOKUP(E59,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M90</v>
+        <v>M150</v>
       </c>
       <c r="N59" t="str">
         <f>LOOKUP(F59,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3620,7 +3685,7 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
@@ -3629,8 +3694,8 @@
         <v>61</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E15-F1-I0-</v>
+        <f>CONCATENATE(A60,"-",B60,"-",C60,"-",D60,"-",E60,"-",F60,"-",G60,"-")</f>
+        <v>A10-C0-D0-L10-E25-F1-I0-</v>
       </c>
       <c r="I60" t="str">
         <f>LOOKUP(A60,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3650,7 +3715,7 @@
       </c>
       <c r="M60" t="str">
         <f>LOOKUP(E60,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M110</v>
+        <v>M150</v>
       </c>
       <c r="N60" t="str">
         <f>LOOKUP(F60,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3665,13 +3730,13 @@
         <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="F61" t="s">
         <v>55</v>
@@ -3680,8 +3745,8 @@
         <v>61</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E15-F1-I0-</v>
+        <f>CONCATENATE(A61,"-",B61,"-",C61,"-",D61,"-",E61,"-",F61,"-",G61,"-")</f>
+        <v>A10-C0-D0-L10-E26-F1-I0-</v>
       </c>
       <c r="I61" t="str">
         <f>LOOKUP(A61,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3693,7 +3758,7 @@
       </c>
       <c r="K61" t="str">
         <f>LOOKUP(C61,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L61" t="str">
         <f>LOOKUP(D61,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3701,7 +3766,7 @@
       </c>
       <c r="M61" t="str">
         <f>LOOKUP(E61,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M110</v>
+        <v>M150</v>
       </c>
       <c r="N61" t="str">
         <f>LOOKUP(F61,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3722,7 +3787,7 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
@@ -3731,8 +3796,8 @@
         <v>61</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E16-F1-I0-</v>
+        <f>CONCATENATE(A62,"-",B62,"-",C62,"-",D62,"-",E62,"-",F62,"-",G62,"-")</f>
+        <v>A10-C0-D0-L10-E27-F1-I0-</v>
       </c>
       <c r="I62" t="str">
         <f>LOOKUP(A62,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3752,7 +3817,7 @@
       </c>
       <c r="M62" t="str">
         <f>LOOKUP(E62,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M120</v>
+        <v>M150</v>
       </c>
       <c r="N62" t="str">
         <f>LOOKUP(F62,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3767,13 +3832,13 @@
         <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -3782,8 +3847,8 @@
         <v>61</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E16-F1-I0-</v>
+        <f>CONCATENATE(A63,"-",B63,"-",C63,"-",D63,"-",E63,"-",F63,"-",G63,"-")</f>
+        <v>A10-C0-D0-L10-E28-F1-I0-</v>
       </c>
       <c r="I63" t="str">
         <f>LOOKUP(A63,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3795,7 +3860,7 @@
       </c>
       <c r="K63" t="str">
         <f>LOOKUP(C63,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
+        <v>no mlacomp</v>
       </c>
       <c r="L63" t="str">
         <f>LOOKUP(D63,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3803,7 +3868,7 @@
       </c>
       <c r="M63" t="str">
         <f>LOOKUP(E63,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M120</v>
+        <v>M150</v>
       </c>
       <c r="N63" t="str">
         <f>LOOKUP(F63,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3824,7 +3889,7 @@
         <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -3833,8 +3898,8 @@
         <v>61</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E17-F1-I0-</v>
+        <f>CONCATENATE(A64,"-",B64,"-",C64,"-",D64,"-",E64,"-",F64,"-",G64,"-")</f>
+        <v>A10-C0-D0-L10-E29-F1-I0-</v>
       </c>
       <c r="I64" t="str">
         <f>LOOKUP(A64,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3854,7 +3919,7 @@
       </c>
       <c r="M64" t="str">
         <f>LOOKUP(E64,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M130</v>
+        <v>M150</v>
       </c>
       <c r="N64" t="str">
         <f>LOOKUP(F64,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3875,7 +3940,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3883,33 +3948,26 @@
       <c r="G65" t="s">
         <v>61</v>
       </c>
-      <c r="H65" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E17-F1-I0-</v>
-      </c>
-      <c r="I65" t="str">
-        <f>LOOKUP(A65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J65" t="str">
-        <f>LOOKUP(B65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K65" t="str">
-        <f>LOOKUP(C65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
-      </c>
-      <c r="L65" t="str">
-        <f>LOOKUP(D65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
-      </c>
-      <c r="M65" t="str">
-        <f>LOOKUP(E65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M130</v>
-      </c>
-      <c r="N65" t="str">
-        <f>LOOKUP(F65,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H65" t="s">
+        <v>64</v>
+      </c>
+      <c r="I65" t="s">
+        <v>9</v>
+      </c>
+      <c r="J65" t="s">
+        <v>12</v>
+      </c>
+      <c r="K65" t="s">
+        <v>14</v>
+      </c>
+      <c r="L65" t="s">
+        <v>16</v>
+      </c>
+      <c r="M65" t="s">
+        <v>48</v>
+      </c>
+      <c r="N65" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -3920,13 +3978,13 @@
         <v>13</v>
       </c>
       <c r="C66" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D66" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F66" t="s">
         <v>55</v>
@@ -3934,38 +3992,31 @@
       <c r="G66" t="s">
         <v>61</v>
       </c>
-      <c r="H66" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E18-F1-I0-</v>
-      </c>
-      <c r="I66" t="str">
-        <f>LOOKUP(A66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J66" t="str">
-        <f>LOOKUP(B66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K66" t="str">
-        <f>LOOKUP(C66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L66" t="str">
-        <f>LOOKUP(D66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
-      </c>
-      <c r="M66" t="str">
-        <f>LOOKUP(E66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M140</v>
-      </c>
-      <c r="N66" t="str">
-        <f>LOOKUP(F66,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H66" t="s">
+        <v>66</v>
+      </c>
+      <c r="I66" t="s">
+        <v>9</v>
+      </c>
+      <c r="J66" t="s">
+        <v>12</v>
+      </c>
+      <c r="K66" t="s">
+        <v>14</v>
+      </c>
+      <c r="L66" t="s">
+        <v>0</v>
+      </c>
+      <c r="M66" t="s">
+        <v>48</v>
+      </c>
+      <c r="N66" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
@@ -3977,7 +4028,7 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F67" t="s">
         <v>55</v>
@@ -3985,50 +4036,43 @@
       <c r="G67" t="s">
         <v>61</v>
       </c>
-      <c r="H67" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E18-F1-I0-</v>
-      </c>
-      <c r="I67" t="str">
-        <f>LOOKUP(A67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J67" t="str">
-        <f>LOOKUP(B67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K67" t="str">
-        <f>LOOKUP(C67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
-      </c>
-      <c r="L67" t="str">
-        <f>LOOKUP(D67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
-      </c>
-      <c r="M67" t="str">
-        <f>LOOKUP(E67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M140</v>
-      </c>
-      <c r="N67" t="str">
-        <f>LOOKUP(F67,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H67" t="s">
+        <v>68</v>
+      </c>
+      <c r="I67" t="s">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>12</v>
+      </c>
+      <c r="K67" t="s">
+        <v>14</v>
+      </c>
+      <c r="L67" t="s">
+        <v>16</v>
+      </c>
+      <c r="M67" t="s">
+        <v>48</v>
+      </c>
+      <c r="N67" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
         <v>13</v>
       </c>
       <c r="C68" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F68" t="s">
         <v>55</v>
@@ -4036,50 +4080,43 @@
       <c r="G68" t="s">
         <v>61</v>
       </c>
-      <c r="H68" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E19-F1-I0-</v>
-      </c>
-      <c r="I68" t="str">
-        <f>LOOKUP(A68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J68" t="str">
-        <f>LOOKUP(B68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K68" t="str">
-        <f>LOOKUP(C68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no mlacomp</v>
-      </c>
-      <c r="L68" t="str">
-        <f>LOOKUP(D68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
-      </c>
-      <c r="M68" t="str">
-        <f>LOOKUP(E68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
-      </c>
-      <c r="N68" t="str">
-        <f>LOOKUP(F68,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H68" t="s">
+        <v>71</v>
+      </c>
+      <c r="I68" t="s">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>12</v>
+      </c>
+      <c r="K68" t="s">
+        <v>14</v>
+      </c>
+      <c r="L68" t="s">
+        <v>0</v>
+      </c>
+      <c r="M68" t="s">
+        <v>48</v>
+      </c>
+      <c r="N68" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
         <v>13</v>
       </c>
       <c r="C69" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F69" t="s">
         <v>55</v>
@@ -4087,37 +4124,39 @@
       <c r="G69" t="s">
         <v>61</v>
       </c>
-      <c r="H69" t="str">
-        <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E19-F1-I0-</v>
-      </c>
-      <c r="I69" t="str">
-        <f>LOOKUP(A69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
-      </c>
-      <c r="J69" t="str">
-        <f>LOOKUP(B69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>no calcomp</v>
-      </c>
-      <c r="K69" t="str">
-        <f>LOOKUP(C69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish mlacomp</v>
-      </c>
-      <c r="L69" t="str">
-        <f>LOOKUP(D69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
-      </c>
-      <c r="M69" t="str">
-        <f>LOOKUP(E69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
-      </c>
-      <c r="N69" t="str">
-        <f>LOOKUP(F69,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>contrast</v>
+      <c r="H69" t="s">
+        <v>72</v>
+      </c>
+      <c r="I69" t="s">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>12</v>
+      </c>
+      <c r="K69" t="s">
+        <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>0</v>
+      </c>
+      <c r="M69" t="s">
+        <v>48</v>
+      </c>
+      <c r="N69" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N49"/>
+  <autoFilter ref="A1:N69">
+    <sortState ref="A2:N69">
+      <sortCondition ref="F2:F69"/>
+      <sortCondition ref="E2:E69"/>
+      <sortCondition ref="B2:B69"/>
+      <sortCondition ref="C2:C69"/>
+      <sortCondition ref="A2:A69"/>
+      <sortCondition ref="D2:D69"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:N49">
     <sortCondition ref="F2:F49"/>
     <sortCondition ref="D2:D49"/>
@@ -4563,7 +4602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -4578,7 +4617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -4593,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
update scenarios, a formula was not working
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\estgrowth\lib\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -14,12 +19,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$69</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="95">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -208,36 +213,6 @@
   </si>
   <si>
     <t>Run make</t>
-  </si>
-  <si>
-    <t>A10-C0-D10-L10-E2-F0-I0-</t>
-  </si>
-  <si>
-    <t>A10-C0-D10-L10-E2-F1-I0-</t>
-  </si>
-  <si>
-    <t>A10-C0-D10-L30-E2-F0-I0-</t>
-  </si>
-  <si>
-    <t>A10-C0-D10-L30-E2-F1-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D10-L10-E2-F0-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D10-L10-E2-F1-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D10-L30-E2-F0-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D20-L30-E2-F0-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D10-L30-E2-F1-I0-</t>
-  </si>
-  <si>
-    <t>A30-C0-D20-L30-E2-F1-I0-</t>
   </si>
   <si>
     <t>E3</t>
@@ -441,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -476,7 +451,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -690,7 +665,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +746,7 @@
         <v>61</v>
       </c>
       <c r="H2" t="str">
-        <f>CONCATENATE(A2,"-",B2,"-",C2,"-",D2,"-",E2,"-",F2,"-",G2,"-")</f>
+        <f t="shared" ref="H2:H65" si="0">CONCATENATE(A2,"-",B2,"-",C2,"-",D2,"-",E2,"-",F2,"-",G2,"-")</f>
         <v>A0-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I2" t="str">
@@ -822,7 +797,7 @@
         <v>61</v>
       </c>
       <c r="H3" t="str">
-        <f>CONCATENATE(A3,"-",B3,"-",C3,"-",D3,"-",E3,"-",F3,"-",G3,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I3" t="str">
@@ -873,7 +848,7 @@
         <v>61</v>
       </c>
       <c r="H4" t="str">
-        <f>CONCATENATE(A4,"-",B4,"-",C4,"-",D4,"-",E4,"-",F4,"-",G4,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I4" t="str">
@@ -924,7 +899,7 @@
         <v>61</v>
       </c>
       <c r="H5" t="str">
-        <f>CONCATENATE(A5,"-",B5,"-",C5,"-",D5,"-",E5,"-",F5,"-",G5,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I5" t="str">
@@ -975,7 +950,7 @@
         <v>61</v>
       </c>
       <c r="H6" t="str">
-        <f>CONCATENATE(A6,"-",B6,"-",C6,"-",D6,"-",E6,"-",F6,"-",G6,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L10-E0-F0-I0-</v>
       </c>
       <c r="I6" t="str">
@@ -1026,7 +1001,7 @@
         <v>61</v>
       </c>
       <c r="H7" t="str">
-        <f>CONCATENATE(A7,"-",B7,"-",C7,"-",D7,"-",E7,"-",F7,"-",G7,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I7" t="str">
@@ -1077,7 +1052,7 @@
         <v>61</v>
       </c>
       <c r="H8" t="str">
-        <f>CONCATENATE(A8,"-",B8,"-",C8,"-",D8,"-",E8,"-",F8,"-",G8,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C20-D0-L30-E0-F0-I0-</v>
       </c>
       <c r="I8" t="str">
@@ -1128,7 +1103,7 @@
         <v>61</v>
       </c>
       <c r="H9" t="str">
-        <f>CONCATENATE(A9,"-",B9,"-",C9,"-",D9,"-",E9,"-",F9,"-",G9,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I9" t="str">
@@ -1179,7 +1154,7 @@
         <v>61</v>
       </c>
       <c r="H10" t="str">
-        <f>CONCATENATE(A10,"-",B10,"-",C10,"-",D10,"-",E10,"-",F10,"-",G10,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I10" t="str">
@@ -1230,7 +1205,7 @@
         <v>61</v>
       </c>
       <c r="H11" t="str">
-        <f>CONCATENATE(A11,"-",B11,"-",C11,"-",D11,"-",E11,"-",F11,"-",G11,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I11" t="str">
@@ -1281,7 +1256,7 @@
         <v>61</v>
       </c>
       <c r="H12" t="str">
-        <f>CONCATENATE(A12,"-",B12,"-",C12,"-",D12,"-",E12,"-",F12,"-",G12,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I12" t="str">
@@ -1332,7 +1307,7 @@
         <v>61</v>
       </c>
       <c r="H13" t="str">
-        <f>CONCATENATE(A13,"-",B13,"-",C13,"-",D13,"-",E13,"-",F13,"-",G13,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L10-E1-F0-I0-</v>
       </c>
       <c r="I13" t="str">
@@ -1383,7 +1358,7 @@
         <v>61</v>
       </c>
       <c r="H14" t="str">
-        <f>CONCATENATE(A14,"-",B14,"-",C14,"-",D14,"-",E14,"-",F14,"-",G14,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I14" t="str">
@@ -1434,7 +1409,7 @@
         <v>61</v>
       </c>
       <c r="H15" t="str">
-        <f>CONCATENATE(A15,"-",B15,"-",C15,"-",D15,"-",E15,"-",F15,"-",G15,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C20-D0-L30-E1-F0-I0-</v>
       </c>
       <c r="I15" t="str">
@@ -1485,7 +1460,7 @@
         <v>61</v>
       </c>
       <c r="H16" t="str">
-        <f>CONCATENATE(A16,"-",B16,"-",C16,"-",D16,"-",E16,"-",F16,"-",G16,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I16" t="str">
@@ -1536,7 +1511,7 @@
         <v>61</v>
       </c>
       <c r="H17" t="str">
-        <f>CONCATENATE(A17,"-",B17,"-",C17,"-",D17,"-",E17,"-",F17,"-",G17,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L30-E2-F0-I0-</v>
       </c>
       <c r="I17" t="str">
@@ -1587,7 +1562,7 @@
         <v>61</v>
       </c>
       <c r="H18" t="str">
-        <f>CONCATENATE(A18,"-",B18,"-",C18,"-",D18,"-",E18,"-",F18,"-",G18,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D10-L10-E2-F0-I0-</v>
       </c>
       <c r="I18" t="str">
@@ -1638,7 +1613,7 @@
         <v>61</v>
       </c>
       <c r="H19" t="str">
-        <f>CONCATENATE(A19,"-",B19,"-",C19,"-",D19,"-",E19,"-",F19,"-",G19,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D10-L30-E2-F0-I0-</v>
       </c>
       <c r="I19" t="str">
@@ -1689,7 +1664,7 @@
         <v>61</v>
       </c>
       <c r="H20" t="str">
-        <f>CONCATENATE(A20,"-",B20,"-",C20,"-",D20,"-",E20,"-",F20,"-",G20,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D20-L30-E2-F0-I0-</v>
       </c>
       <c r="I20" t="str">
@@ -1731,7 +1706,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
         <v>54</v>
@@ -1739,8 +1714,9 @@
       <c r="G21" t="s">
         <v>61</v>
       </c>
-      <c r="H21" t="s">
-        <v>63</v>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E3-F0-I0-</v>
       </c>
       <c r="I21" t="s">
         <v>9</v>
@@ -1775,7 +1751,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
         <v>54</v>
@@ -1783,8 +1759,9 @@
       <c r="G22" t="s">
         <v>61</v>
       </c>
-      <c r="H22" t="s">
-        <v>65</v>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L30-E3-F0-I0-</v>
       </c>
       <c r="I22" t="s">
         <v>9</v>
@@ -1819,7 +1796,7 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
         <v>54</v>
@@ -1827,8 +1804,9 @@
       <c r="G23" t="s">
         <v>61</v>
       </c>
-      <c r="H23" t="s">
-        <v>67</v>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>A30-C0-D10-L10-E3-F0-I0-</v>
       </c>
       <c r="I23" t="s">
         <v>0</v>
@@ -1863,7 +1841,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
         <v>54</v>
@@ -1871,8 +1849,9 @@
       <c r="G24" t="s">
         <v>61</v>
       </c>
-      <c r="H24" t="s">
-        <v>69</v>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>A30-C0-D10-L30-E3-F0-I0-</v>
       </c>
       <c r="I24" t="s">
         <v>0</v>
@@ -1907,7 +1886,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
         <v>54</v>
@@ -1915,8 +1894,9 @@
       <c r="G25" t="s">
         <v>61</v>
       </c>
-      <c r="H25" t="s">
-        <v>70</v>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>A30-C0-D20-L30-E3-F0-I0-</v>
       </c>
       <c r="I25" t="s">
         <v>0</v>
@@ -1960,7 +1940,7 @@
         <v>61</v>
       </c>
       <c r="H26" t="str">
-        <f>CONCATENATE(A26,"-",B26,"-",C26,"-",D26,"-",E26,"-",F26,"-",G26,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I26" t="str">
@@ -2011,7 +1991,7 @@
         <v>61</v>
       </c>
       <c r="H27" t="str">
-        <f>CONCATENATE(A27,"-",B27,"-",C27,"-",D27,"-",E27,"-",F27,"-",G27,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I27" t="str">
@@ -2062,7 +2042,7 @@
         <v>61</v>
       </c>
       <c r="H28" t="str">
-        <f>CONCATENATE(A28,"-",B28,"-",C28,"-",D28,"-",E28,"-",F28,"-",G28,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I28" t="str">
@@ -2113,7 +2093,7 @@
         <v>61</v>
       </c>
       <c r="H29" t="str">
-        <f>CONCATENATE(A29,"-",B29,"-",C29,"-",D29,"-",E29,"-",F29,"-",G29,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I29" t="str">
@@ -2164,7 +2144,7 @@
         <v>61</v>
       </c>
       <c r="H30" t="str">
-        <f>CONCATENATE(A30,"-",B30,"-",C30,"-",D30,"-",E30,"-",F30,"-",G30,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L10-E0-F1-I0-</v>
       </c>
       <c r="I30" t="str">
@@ -2215,7 +2195,7 @@
         <v>61</v>
       </c>
       <c r="H31" t="str">
-        <f>CONCATENATE(A31,"-",B31,"-",C31,"-",D31,"-",E31,"-",F31,"-",G31,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I31" t="str">
@@ -2266,7 +2246,7 @@
         <v>61</v>
       </c>
       <c r="H32" t="str">
-        <f>CONCATENATE(A32,"-",B32,"-",C32,"-",D32,"-",E32,"-",F32,"-",G32,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C20-D0-L30-E0-F1-I0-</v>
       </c>
       <c r="I32" t="str">
@@ -2317,7 +2297,7 @@
         <v>61</v>
       </c>
       <c r="H33" t="str">
-        <f>CONCATENATE(A33,"-",B33,"-",C33,"-",D33,"-",E33,"-",F33,"-",G33,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I33" t="str">
@@ -2368,7 +2348,7 @@
         <v>61</v>
       </c>
       <c r="H34" t="str">
-        <f>CONCATENATE(A34,"-",B34,"-",C34,"-",D34,"-",E34,"-",F34,"-",G34,"-")</f>
+        <f t="shared" si="0"/>
         <v>A0-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I34" t="str">
@@ -2419,7 +2399,7 @@
         <v>61</v>
       </c>
       <c r="H35" t="str">
-        <f>CONCATENATE(A35,"-",B35,"-",C35,"-",D35,"-",E35,"-",F35,"-",G35,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I35" t="str">
@@ -2470,7 +2450,7 @@
         <v>61</v>
       </c>
       <c r="H36" t="str">
-        <f>CONCATENATE(A36,"-",B36,"-",C36,"-",D36,"-",E36,"-",F36,"-",G36,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I36" t="str">
@@ -2521,7 +2501,7 @@
         <v>61</v>
       </c>
       <c r="H37" t="str">
-        <f>CONCATENATE(A37,"-",B37,"-",C37,"-",D37,"-",E37,"-",F37,"-",G37,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L10-E1-F1-I0-</v>
       </c>
       <c r="I37" t="str">
@@ -2572,7 +2552,7 @@
         <v>61</v>
       </c>
       <c r="H38" t="str">
-        <f>CONCATENATE(A38,"-",B38,"-",C38,"-",D38,"-",E38,"-",F38,"-",G38,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I38" t="str">
@@ -2623,7 +2603,7 @@
         <v>61</v>
       </c>
       <c r="H39" t="str">
-        <f>CONCATENATE(A39,"-",B39,"-",C39,"-",D39,"-",E39,"-",F39,"-",G39,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C20-D0-L30-E1-F1-I0-</v>
       </c>
       <c r="I39" t="str">
@@ -2665,7 +2645,7 @@
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="F40" t="s">
         <v>55</v>
@@ -2674,7 +2654,7 @@
         <v>61</v>
       </c>
       <c r="H40" t="str">
-        <f>CONCATENATE(A40,"-",B40,"-",C40,"-",D40,"-",E40,"-",F40,"-",G40,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E10-F1-I0-</v>
       </c>
       <c r="I40" t="str">
@@ -2716,7 +2696,7 @@
         <v>17</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F41" t="s">
         <v>55</v>
@@ -2725,7 +2705,7 @@
         <v>61</v>
       </c>
       <c r="H41" t="str">
-        <f>CONCATENATE(A41,"-",B41,"-",C41,"-",D41,"-",E41,"-",F41,"-",G41,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E11-F1-I0-</v>
       </c>
       <c r="I41" t="str">
@@ -2767,7 +2747,7 @@
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F42" t="s">
         <v>55</v>
@@ -2776,7 +2756,7 @@
         <v>61</v>
       </c>
       <c r="H42" t="str">
-        <f>CONCATENATE(A42,"-",B42,"-",C42,"-",D42,"-",E42,"-",F42,"-",G42,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E12-F1-I0-</v>
       </c>
       <c r="I42" t="str">
@@ -2818,7 +2798,7 @@
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F43" t="s">
         <v>55</v>
@@ -2827,7 +2807,7 @@
         <v>61</v>
       </c>
       <c r="H43" t="str">
-        <f>CONCATENATE(A43,"-",B43,"-",C43,"-",D43,"-",E43,"-",F43,"-",G43,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E13-F1-I0-</v>
       </c>
       <c r="I43" t="str">
@@ -2869,7 +2849,7 @@
         <v>17</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="F44" t="s">
         <v>55</v>
@@ -2878,7 +2858,7 @@
         <v>61</v>
       </c>
       <c r="H44" t="str">
-        <f>CONCATENATE(A44,"-",B44,"-",C44,"-",D44,"-",E44,"-",F44,"-",G44,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E14-F1-I0-</v>
       </c>
       <c r="I44" t="str">
@@ -2920,7 +2900,7 @@
         <v>17</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F45" t="s">
         <v>55</v>
@@ -2929,7 +2909,7 @@
         <v>61</v>
       </c>
       <c r="H45" t="str">
-        <f>CONCATENATE(A45,"-",B45,"-",C45,"-",D45,"-",E45,"-",F45,"-",G45,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E15-F1-I0-</v>
       </c>
       <c r="I45" t="str">
@@ -2971,7 +2951,7 @@
         <v>17</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F46" t="s">
         <v>55</v>
@@ -2980,7 +2960,7 @@
         <v>61</v>
       </c>
       <c r="H46" t="str">
-        <f>CONCATENATE(A46,"-",B46,"-",C46,"-",D46,"-",E46,"-",F46,"-",G46,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E16-F1-I0-</v>
       </c>
       <c r="I46" t="str">
@@ -3022,7 +3002,7 @@
         <v>17</v>
       </c>
       <c r="E47" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
         <v>55</v>
@@ -3031,7 +3011,7 @@
         <v>61</v>
       </c>
       <c r="H47" t="str">
-        <f>CONCATENATE(A47,"-",B47,"-",C47,"-",D47,"-",E47,"-",F47,"-",G47,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E17-F1-I0-</v>
       </c>
       <c r="I47" t="str">
@@ -3073,7 +3053,7 @@
         <v>17</v>
       </c>
       <c r="E48" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F48" t="s">
         <v>55</v>
@@ -3082,7 +3062,7 @@
         <v>61</v>
       </c>
       <c r="H48" t="str">
-        <f>CONCATENATE(A48,"-",B48,"-",C48,"-",D48,"-",E48,"-",F48,"-",G48,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E18-F1-I0-</v>
       </c>
       <c r="I48" t="str">
@@ -3124,7 +3104,7 @@
         <v>17</v>
       </c>
       <c r="E49" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F49" t="s">
         <v>55</v>
@@ -3133,7 +3113,7 @@
         <v>61</v>
       </c>
       <c r="H49" t="str">
-        <f>CONCATENATE(A49,"-",B49,"-",C49,"-",D49,"-",E49,"-",F49,"-",G49,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E19-F1-I0-</v>
       </c>
       <c r="I49" t="str">
@@ -3184,7 +3164,7 @@
         <v>61</v>
       </c>
       <c r="H50" t="str">
-        <f>CONCATENATE(A50,"-",B50,"-",C50,"-",D50,"-",E50,"-",F50,"-",G50,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I50" t="str">
@@ -3235,7 +3215,7 @@
         <v>61</v>
       </c>
       <c r="H51" t="str">
-        <f>CONCATENATE(A51,"-",B51,"-",C51,"-",D51,"-",E51,"-",F51,"-",G51,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D10-L30-E2-F1-I0-</v>
       </c>
       <c r="I51" t="str">
@@ -3286,7 +3266,7 @@
         <v>61</v>
       </c>
       <c r="H52" t="str">
-        <f>CONCATENATE(A52,"-",B52,"-",C52,"-",D52,"-",E52,"-",F52,"-",G52,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D10-L10-E2-F1-I0-</v>
       </c>
       <c r="I52" t="str">
@@ -3337,7 +3317,7 @@
         <v>61</v>
       </c>
       <c r="H53" t="str">
-        <f>CONCATENATE(A53,"-",B53,"-",C53,"-",D53,"-",E53,"-",F53,"-",G53,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D10-L30-E2-F1-I0-</v>
       </c>
       <c r="I53" t="str">
@@ -3388,7 +3368,7 @@
         <v>61</v>
       </c>
       <c r="H54" t="str">
-        <f>CONCATENATE(A54,"-",B54,"-",C54,"-",D54,"-",E54,"-",F54,"-",G54,"-")</f>
+        <f t="shared" si="0"/>
         <v>A30-C0-D20-L30-E2-F1-I0-</v>
       </c>
       <c r="I54" t="str">
@@ -3430,7 +3410,7 @@
         <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -3439,7 +3419,7 @@
         <v>61</v>
       </c>
       <c r="H55" t="str">
-        <f>CONCATENATE(A55,"-",B55,"-",C55,"-",D55,"-",E55,"-",F55,"-",G55,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E20-F1-I0-</v>
       </c>
       <c r="I55" t="str">
@@ -3481,7 +3461,7 @@
         <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
@@ -3490,7 +3470,7 @@
         <v>61</v>
       </c>
       <c r="H56" t="str">
-        <f>CONCATENATE(A56,"-",B56,"-",C56,"-",D56,"-",E56,"-",F56,"-",G56,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E21-F1-I0-</v>
       </c>
       <c r="I56" t="str">
@@ -3532,7 +3512,7 @@
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
@@ -3541,7 +3521,7 @@
         <v>61</v>
       </c>
       <c r="H57" t="str">
-        <f>CONCATENATE(A57,"-",B57,"-",C57,"-",D57,"-",E57,"-",F57,"-",G57,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E22-F1-I0-</v>
       </c>
       <c r="I57" t="str">
@@ -3583,7 +3563,7 @@
         <v>17</v>
       </c>
       <c r="E58" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
@@ -3592,7 +3572,7 @@
         <v>61</v>
       </c>
       <c r="H58" t="str">
-        <f>CONCATENATE(A58,"-",B58,"-",C58,"-",D58,"-",E58,"-",F58,"-",G58,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E23-F1-I0-</v>
       </c>
       <c r="I58" t="str">
@@ -3634,7 +3614,7 @@
         <v>17</v>
       </c>
       <c r="E59" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
@@ -3643,7 +3623,7 @@
         <v>61</v>
       </c>
       <c r="H59" t="str">
-        <f>CONCATENATE(A59,"-",B59,"-",C59,"-",D59,"-",E59,"-",F59,"-",G59,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E24-F1-I0-</v>
       </c>
       <c r="I59" t="str">
@@ -3685,7 +3665,7 @@
         <v>17</v>
       </c>
       <c r="E60" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
@@ -3694,7 +3674,7 @@
         <v>61</v>
       </c>
       <c r="H60" t="str">
-        <f>CONCATENATE(A60,"-",B60,"-",C60,"-",D60,"-",E60,"-",F60,"-",G60,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E25-F1-I0-</v>
       </c>
       <c r="I60" t="str">
@@ -3736,7 +3716,7 @@
         <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F61" t="s">
         <v>55</v>
@@ -3745,7 +3725,7 @@
         <v>61</v>
       </c>
       <c r="H61" t="str">
-        <f>CONCATENATE(A61,"-",B61,"-",C61,"-",D61,"-",E61,"-",F61,"-",G61,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E26-F1-I0-</v>
       </c>
       <c r="I61" t="str">
@@ -3787,7 +3767,7 @@
         <v>17</v>
       </c>
       <c r="E62" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
@@ -3796,7 +3776,7 @@
         <v>61</v>
       </c>
       <c r="H62" t="str">
-        <f>CONCATENATE(A62,"-",B62,"-",C62,"-",D62,"-",E62,"-",F62,"-",G62,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E27-F1-I0-</v>
       </c>
       <c r="I62" t="str">
@@ -3838,7 +3818,7 @@
         <v>17</v>
       </c>
       <c r="E63" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -3847,7 +3827,7 @@
         <v>61</v>
       </c>
       <c r="H63" t="str">
-        <f>CONCATENATE(A63,"-",B63,"-",C63,"-",D63,"-",E63,"-",F63,"-",G63,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E28-F1-I0-</v>
       </c>
       <c r="I63" t="str">
@@ -3889,7 +3869,7 @@
         <v>17</v>
       </c>
       <c r="E64" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -3898,7 +3878,7 @@
         <v>61</v>
       </c>
       <c r="H64" t="str">
-        <f>CONCATENATE(A64,"-",B64,"-",C64,"-",D64,"-",E64,"-",F64,"-",G64,"-")</f>
+        <f t="shared" si="0"/>
         <v>A10-C0-D0-L10-E29-F1-I0-</v>
       </c>
       <c r="I64" t="str">
@@ -3940,7 +3920,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3948,8 +3928,9 @@
       <c r="G65" t="s">
         <v>61</v>
       </c>
-      <c r="H65" t="s">
-        <v>64</v>
+      <c r="H65" t="str">
+        <f t="shared" si="0"/>
+        <v>A10-C0-D10-L10-E3-F1-I0-</v>
       </c>
       <c r="I65" t="s">
         <v>9</v>
@@ -3984,7 +3965,7 @@
         <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F66" t="s">
         <v>55</v>
@@ -3992,8 +3973,9 @@
       <c r="G66" t="s">
         <v>61</v>
       </c>
-      <c r="H66" t="s">
-        <v>66</v>
+      <c r="H66" t="str">
+        <f t="shared" ref="H66:H69" si="1">CONCATENATE(A66,"-",B66,"-",C66,"-",D66,"-",E66,"-",F66,"-",G66,"-")</f>
+        <v>A10-C0-D10-L30-E3-F1-I0-</v>
       </c>
       <c r="I66" t="s">
         <v>9</v>
@@ -4028,7 +4010,7 @@
         <v>17</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F67" t="s">
         <v>55</v>
@@ -4036,8 +4018,9 @@
       <c r="G67" t="s">
         <v>61</v>
       </c>
-      <c r="H67" t="s">
-        <v>68</v>
+      <c r="H67" t="str">
+        <f t="shared" si="1"/>
+        <v>A30-C0-D10-L10-E3-F1-I0-</v>
       </c>
       <c r="I67" t="s">
         <v>0</v>
@@ -4072,7 +4055,7 @@
         <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F68" t="s">
         <v>55</v>
@@ -4080,8 +4063,9 @@
       <c r="G68" t="s">
         <v>61</v>
       </c>
-      <c r="H68" t="s">
-        <v>71</v>
+      <c r="H68" t="str">
+        <f t="shared" si="1"/>
+        <v>A30-C0-D10-L30-E3-F1-I0-</v>
       </c>
       <c r="I68" t="s">
         <v>0</v>
@@ -4116,7 +4100,7 @@
         <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F69" t="s">
         <v>55</v>
@@ -4124,8 +4108,9 @@
       <c r="G69" t="s">
         <v>61</v>
       </c>
-      <c r="H69" t="s">
-        <v>72</v>
+      <c r="H69" t="str">
+        <f t="shared" si="1"/>
+        <v>A30-C0-D20-L30-E3-F1-I0-</v>
       </c>
       <c r="I69" t="s">
         <v>0</v>
@@ -4404,7 +4389,7 @@
         <v>E3</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -4419,7 +4404,7 @@
         <v>E10</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4434,7 +4419,7 @@
         <v>E11</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4449,7 +4434,7 @@
         <v>E12</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -4464,7 +4449,7 @@
         <v>E13</v>
       </c>
       <c r="D19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -4479,7 +4464,7 @@
         <v>E14</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4494,7 +4479,7 @@
         <v>E15</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -4509,7 +4494,7 @@
         <v>E16</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -4524,7 +4509,7 @@
         <v>E17</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -4539,7 +4524,7 @@
         <v>E18</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -4554,7 +4539,7 @@
         <v>E19</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Modify cases for no survey selectivity if no survey data
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\estgrowth\lib\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
@@ -19,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenarios!$A$1:$N$69</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="99">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -309,6 +304,18 @@
   </si>
   <si>
     <t>E29</t>
+  </si>
+  <si>
+    <t>E100</t>
+  </si>
+  <si>
+    <t>E101</t>
+  </si>
+  <si>
+    <t>E102</t>
+  </si>
+  <si>
+    <t>E103</t>
   </si>
 </sst>
 </file>
@@ -416,7 +423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,7 +458,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,7 +672,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +744,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>
@@ -747,7 +754,7 @@
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H65" si="0">CONCATENATE(A2,"-",B2,"-",C2,"-",D2,"-",E2,"-",F2,"-",G2,"-")</f>
-        <v>A0-C0-D0-L10-E0-F0-I0-</v>
+        <v>A0-C0-D0-L10-E100-F0-I0-</v>
       </c>
       <c r="I2" t="str">
         <f>LOOKUP(A2,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -767,7 +774,7 @@
       </c>
       <c r="M2" t="str">
         <f>LOOKUP(E2,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M50</v>
       </c>
       <c r="N2" t="str">
         <f>LOOKUP(F2,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -839,7 +846,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -849,7 +856,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E0-F0-I0-</v>
+        <v>A10-C0-D0-L10-E100-F0-I0-</v>
       </c>
       <c r="I4" t="str">
         <f>LOOKUP(A4,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -869,7 +876,7 @@
       </c>
       <c r="M4" t="str">
         <f>LOOKUP(E4,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M50</v>
       </c>
       <c r="N4" t="str">
         <f>LOOKUP(F4,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1094,7 +1101,7 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -1104,7 +1111,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E1-F0-I0-</v>
+        <v>A0-C0-D0-L10-E101-F0-I0-</v>
       </c>
       <c r="I9" t="str">
         <f>LOOKUP(A9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1124,7 +1131,7 @@
       </c>
       <c r="M9" t="str">
         <f>LOOKUP(E9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M50</v>
       </c>
       <c r="N9" t="str">
         <f>LOOKUP(F9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1196,7 +1203,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
@@ -1206,7 +1213,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E1-F0-I0-</v>
+        <v>A10-C0-D0-L10-E101-F0-I0-</v>
       </c>
       <c r="I11" t="str">
         <f>LOOKUP(A11,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1226,7 +1233,7 @@
       </c>
       <c r="M11" t="str">
         <f>LOOKUP(E11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M50</v>
       </c>
       <c r="N11" t="str">
         <f>LOOKUP(F11,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1451,7 +1458,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F16" t="s">
         <v>54</v>
@@ -1461,7 +1468,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E2-F0-I0-</v>
+        <v>A10-C0-D10-L10-E102-F0-I0-</v>
       </c>
       <c r="I16" t="str">
         <f>LOOKUP(A16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1481,7 +1488,7 @@
       </c>
       <c r="M16" t="str">
         <f>LOOKUP(E16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>M50</v>
       </c>
       <c r="N16" t="str">
         <f>LOOKUP(F16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1706,7 +1713,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
         <v>54</v>
@@ -1716,7 +1723,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E3-F0-I0-</v>
+        <v>A10-C0-D10-L10-E103-F0-I0-</v>
       </c>
       <c r="I21" t="s">
         <v>9</v>
@@ -1931,7 +1938,7 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
         <v>55</v>
@@ -1941,7 +1948,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E0-F1-I0-</v>
+        <v>A0-C0-D0-L10-E100-F1-I0-</v>
       </c>
       <c r="I26" t="str">
         <f>LOOKUP(A26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1961,7 +1968,7 @@
       </c>
       <c r="M26" t="str">
         <f>LOOKUP(E26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M50</v>
       </c>
       <c r="N26" t="str">
         <f>LOOKUP(F26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2033,7 +2040,7 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -2043,7 +2050,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E0-F1-I0-</v>
+        <v>A10-C0-D0-L10-E100-F1-I0-</v>
       </c>
       <c r="I28" t="str">
         <f>LOOKUP(A28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2063,7 +2070,7 @@
       </c>
       <c r="M28" t="str">
         <f>LOOKUP(E28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fixed</v>
+        <v>M50</v>
       </c>
       <c r="N28" t="str">
         <f>LOOKUP(F28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2288,7 +2295,7 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
@@ -2298,7 +2305,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>A0-C0-D0-L10-E1-F1-I0-</v>
+        <v>A0-C0-D0-L10-E101-F1-I0-</v>
       </c>
       <c r="I33" t="str">
         <f>LOOKUP(A33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2318,7 +2325,7 @@
       </c>
       <c r="M33" t="str">
         <f>LOOKUP(E33,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M50</v>
       </c>
       <c r="N33" t="str">
         <f>LOOKUP(F33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2390,7 +2397,7 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F35" t="s">
         <v>55</v>
@@ -2400,7 +2407,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E1-F1-I0-</v>
+        <v>A10-C0-D0-L10-E101-F1-I0-</v>
       </c>
       <c r="I35" t="str">
         <f>LOOKUP(A35,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2420,7 +2427,7 @@
       </c>
       <c r="M35" t="str">
         <f>LOOKUP(E35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>internal</v>
+        <v>M50</v>
       </c>
       <c r="N35" t="str">
         <f>LOOKUP(F35,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3155,7 +3162,7 @@
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
         <v>55</v>
@@ -3165,7 +3172,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E2-F1-I0-</v>
+        <v>A10-C0-D10-L10-E102-F1-I0-</v>
       </c>
       <c r="I50" t="str">
         <f>LOOKUP(A50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3185,7 +3192,7 @@
       </c>
       <c r="M50" t="str">
         <f>LOOKUP(E50,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>M50</v>
       </c>
       <c r="N50" t="str">
         <f>LOOKUP(F50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3920,7 +3927,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -3930,7 +3937,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E3-F1-I0-</v>
+        <v>A10-C0-D10-L10-E103-F1-I0-</v>
       </c>
       <c r="I65" t="s">
         <v>9</v>
@@ -4132,16 +4139,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N69">
-    <sortState ref="A2:N69">
-      <sortCondition ref="F2:F69"/>
-      <sortCondition ref="E2:E69"/>
-      <sortCondition ref="B2:B69"/>
-      <sortCondition ref="C2:C69"/>
-      <sortCondition ref="A2:A69"/>
-      <sortCondition ref="D2:D69"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:N69"/>
   <sortState ref="A2:N49">
     <sortCondition ref="F2:F49"/>
     <sortCondition ref="D2:D49"/>

</xml_diff>

<commit_message>
Change range of M to also use survey data
</commit_message>
<xml_diff>
--- a/lib/scenarios.xlsx
+++ b/lib/scenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="89">
   <si>
     <t>fish &amp; surv length</t>
   </si>
@@ -244,36 +244,6 @@
   </si>
   <si>
     <t>internalCV</t>
-  </si>
-  <si>
-    <t>M60</t>
-  </si>
-  <si>
-    <t>M80</t>
-  </si>
-  <si>
-    <t>M50</t>
-  </si>
-  <si>
-    <t>M70</t>
-  </si>
-  <si>
-    <t>M90</t>
-  </si>
-  <si>
-    <t>M110</t>
-  </si>
-  <si>
-    <t>M120</t>
-  </si>
-  <si>
-    <t>M130</t>
-  </si>
-  <si>
-    <t>M140</t>
-  </si>
-  <si>
-    <t>M150</t>
   </si>
   <si>
     <t>E20</t>
@@ -744,7 +714,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>
@@ -774,7 +744,7 @@
       </c>
       <c r="M2" t="str">
         <f>LOOKUP(E2,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N2" t="str">
         <f>LOOKUP(F2,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -846,7 +816,7 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
@@ -876,7 +846,7 @@
       </c>
       <c r="M4" t="str">
         <f>LOOKUP(E4,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N4" t="str">
         <f>LOOKUP(F4,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1101,7 +1071,7 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
@@ -1131,7 +1101,7 @@
       </c>
       <c r="M9" t="str">
         <f>LOOKUP(E9,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N9" t="str">
         <f>LOOKUP(F9,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1203,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
@@ -1233,7 +1203,7 @@
       </c>
       <c r="M11" t="str">
         <f>LOOKUP(E11,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N11" t="str">
         <f>LOOKUP(F11,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1458,7 +1428,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
         <v>54</v>
@@ -1488,7 +1458,7 @@
       </c>
       <c r="M16" t="str">
         <f>LOOKUP(E16,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N16" t="str">
         <f>LOOKUP(F16,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1539,7 +1509,7 @@
       </c>
       <c r="M17" t="str">
         <f>LOOKUP(E17,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N17" t="str">
         <f>LOOKUP(F17,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1590,7 +1560,7 @@
       </c>
       <c r="M18" t="str">
         <f>LOOKUP(E18,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N18" t="str">
         <f>LOOKUP(F18,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1641,7 +1611,7 @@
       </c>
       <c r="M19" t="str">
         <f>LOOKUP(E19,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N19" t="str">
         <f>LOOKUP(F19,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1692,7 +1662,7 @@
       </c>
       <c r="M20" t="str">
         <f>LOOKUP(E20,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N20" t="str">
         <f>LOOKUP(F20,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -1713,7 +1683,7 @@
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
         <v>54</v>
@@ -1938,7 +1908,7 @@
         <v>17</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F26" t="s">
         <v>55</v>
@@ -1968,7 +1938,7 @@
       </c>
       <c r="M26" t="str">
         <f>LOOKUP(E26,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N26" t="str">
         <f>LOOKUP(F26,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2040,7 +2010,7 @@
         <v>17</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
         <v>55</v>
@@ -2070,7 +2040,7 @@
       </c>
       <c r="M28" t="str">
         <f>LOOKUP(E28,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N28" t="str">
         <f>LOOKUP(F28,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2295,7 +2265,7 @@
         <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
@@ -2325,7 +2295,7 @@
       </c>
       <c r="M33" t="str">
         <f>LOOKUP(E33,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N33" t="str">
         <f>LOOKUP(F33,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2397,7 +2367,7 @@
         <v>17</v>
       </c>
       <c r="E35" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
         <v>55</v>
@@ -2427,7 +2397,7 @@
       </c>
       <c r="M35" t="str">
         <f>LOOKUP(E35,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N35" t="str">
         <f>LOOKUP(F35,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2640,7 +2610,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
@@ -2649,7 +2619,7 @@
         <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
         <v>64</v>
@@ -2662,11 +2632,11 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E10-F1-I0-</v>
+        <v>A30-C0-D10-L30-E10-F1-I0-</v>
       </c>
       <c r="I40" t="str">
         <f>LOOKUP(A40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J40" t="str">
         <f>LOOKUP(B40,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2678,11 +2648,11 @@
       </c>
       <c r="L40" t="str">
         <f>LOOKUP(D40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M40" t="str">
         <f>LOOKUP(E40,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N40" t="str">
         <f>LOOKUP(F40,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2691,7 +2661,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
         <v>13</v>
@@ -2700,7 +2670,7 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
         <v>65</v>
@@ -2713,11 +2683,11 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E11-F1-I0-</v>
+        <v>A30-C0-D10-L30-E11-F1-I0-</v>
       </c>
       <c r="I41" t="str">
         <f>LOOKUP(A41,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J41" t="str">
         <f>LOOKUP(B41,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2729,11 +2699,11 @@
       </c>
       <c r="L41" t="str">
         <f>LOOKUP(D41,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M41" t="str">
         <f>LOOKUP(E41,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M60</v>
+        <v>external</v>
       </c>
       <c r="N41" t="str">
         <f>LOOKUP(F41,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2742,7 +2712,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -2751,7 +2721,7 @@
         <v>15</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
         <v>66</v>
@@ -2764,11 +2734,11 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E12-F1-I0-</v>
+        <v>A30-C0-D10-L30-E12-F1-I0-</v>
       </c>
       <c r="I42" t="str">
         <f>LOOKUP(A42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J42" t="str">
         <f>LOOKUP(B42,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2780,11 +2750,11 @@
       </c>
       <c r="L42" t="str">
         <f>LOOKUP(D42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M42" t="str">
         <f>LOOKUP(E42,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M70</v>
+        <v>external</v>
       </c>
       <c r="N42" t="str">
         <f>LOOKUP(F42,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2793,7 +2763,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
@@ -2802,7 +2772,7 @@
         <v>15</v>
       </c>
       <c r="D43" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
         <v>67</v>
@@ -2815,11 +2785,11 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E13-F1-I0-</v>
+        <v>A30-C0-D10-L30-E13-F1-I0-</v>
       </c>
       <c r="I43" t="str">
         <f>LOOKUP(A43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J43" t="str">
         <f>LOOKUP(B43,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2831,11 +2801,11 @@
       </c>
       <c r="L43" t="str">
         <f>LOOKUP(D43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M43" t="str">
         <f>LOOKUP(E43,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M80</v>
+        <v>external</v>
       </c>
       <c r="N43" t="str">
         <f>LOOKUP(F43,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2844,7 +2814,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
         <v>13</v>
@@ -2853,7 +2823,7 @@
         <v>15</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
         <v>68</v>
@@ -2866,11 +2836,11 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E14-F1-I0-</v>
+        <v>A30-C0-D10-L30-E14-F1-I0-</v>
       </c>
       <c r="I44" t="str">
         <f>LOOKUP(A44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J44" t="str">
         <f>LOOKUP(B44,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2882,11 +2852,11 @@
       </c>
       <c r="L44" t="str">
         <f>LOOKUP(D44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M44" t="str">
         <f>LOOKUP(E44,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M90</v>
+        <v>external</v>
       </c>
       <c r="N44" t="str">
         <f>LOOKUP(F44,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2895,7 +2865,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
         <v>13</v>
@@ -2904,7 +2874,7 @@
         <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
         <v>69</v>
@@ -2917,11 +2887,11 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E15-F1-I0-</v>
+        <v>A30-C0-D10-L30-E15-F1-I0-</v>
       </c>
       <c r="I45" t="str">
         <f>LOOKUP(A45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J45" t="str">
         <f>LOOKUP(B45,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2933,11 +2903,11 @@
       </c>
       <c r="L45" t="str">
         <f>LOOKUP(D45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M45" t="str">
         <f>LOOKUP(E45,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M110</v>
+        <v>external</v>
       </c>
       <c r="N45" t="str">
         <f>LOOKUP(F45,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2946,7 +2916,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -2955,7 +2925,7 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
         <v>70</v>
@@ -2968,11 +2938,11 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E16-F1-I0-</v>
+        <v>A30-C0-D10-L30-E16-F1-I0-</v>
       </c>
       <c r="I46" t="str">
         <f>LOOKUP(A46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J46" t="str">
         <f>LOOKUP(B46,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2984,11 +2954,11 @@
       </c>
       <c r="L46" t="str">
         <f>LOOKUP(D46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M46" t="str">
         <f>LOOKUP(E46,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M120</v>
+        <v>external</v>
       </c>
       <c r="N46" t="str">
         <f>LOOKUP(F46,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -2997,7 +2967,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
@@ -3006,7 +2976,7 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
         <v>71</v>
@@ -3019,11 +2989,11 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E17-F1-I0-</v>
+        <v>A30-C0-D10-L30-E17-F1-I0-</v>
       </c>
       <c r="I47" t="str">
         <f>LOOKUP(A47,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J47" t="str">
         <f>LOOKUP(B47,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3035,11 +3005,11 @@
       </c>
       <c r="L47" t="str">
         <f>LOOKUP(D47,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M47" t="str">
         <f>LOOKUP(E47,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M130</v>
+        <v>external</v>
       </c>
       <c r="N47" t="str">
         <f>LOOKUP(F47,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3048,7 +3018,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s">
         <v>13</v>
@@ -3057,7 +3027,7 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
         <v>72</v>
@@ -3070,11 +3040,11 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E18-F1-I0-</v>
+        <v>A30-C0-D10-L30-E18-F1-I0-</v>
       </c>
       <c r="I48" t="str">
         <f>LOOKUP(A48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J48" t="str">
         <f>LOOKUP(B48,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3086,11 +3056,11 @@
       </c>
       <c r="L48" t="str">
         <f>LOOKUP(D48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M48" t="str">
         <f>LOOKUP(E48,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M140</v>
+        <v>external</v>
       </c>
       <c r="N48" t="str">
         <f>LOOKUP(F48,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3099,7 +3069,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B49" t="s">
         <v>13</v>
@@ -3108,7 +3078,7 @@
         <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
         <v>73</v>
@@ -3121,11 +3091,11 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D10-L10-E19-F1-I0-</v>
+        <v>A30-C0-D10-L30-E19-F1-I0-</v>
       </c>
       <c r="I49" t="str">
         <f>LOOKUP(A49,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J49" t="str">
         <f>LOOKUP(B49,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3137,11 +3107,11 @@
       </c>
       <c r="L49" t="str">
         <f>LOOKUP(D49,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M49" t="str">
         <f>LOOKUP(E49,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N49" t="str">
         <f>LOOKUP(F49,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3162,7 +3132,7 @@
         <v>17</v>
       </c>
       <c r="E50" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="F50" t="s">
         <v>55</v>
@@ -3192,7 +3162,7 @@
       </c>
       <c r="M50" t="str">
         <f>LOOKUP(E50,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M50</v>
+        <v>external</v>
       </c>
       <c r="N50" t="str">
         <f>LOOKUP(F50,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3243,7 +3213,7 @@
       </c>
       <c r="M51" t="str">
         <f>LOOKUP(E51,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N51" t="str">
         <f>LOOKUP(F51,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3294,7 +3264,7 @@
       </c>
       <c r="M52" t="str">
         <f>LOOKUP(E52,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N52" t="str">
         <f>LOOKUP(F52,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3345,7 +3315,7 @@
       </c>
       <c r="M53" t="str">
         <f>LOOKUP(E53,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N53" t="str">
         <f>LOOKUP(F53,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3396,7 +3366,7 @@
       </c>
       <c r="M54" t="str">
         <f>LOOKUP(E54,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>external</v>
       </c>
       <c r="N54" t="str">
         <f>LOOKUP(F54,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3405,7 +3375,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
         <v>13</v>
@@ -3414,10 +3384,10 @@
         <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F55" t="s">
         <v>55</v>
@@ -3427,11 +3397,11 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E20-F1-I0-</v>
+        <v>A30-C0-D0-L30-E20-F1-I0-</v>
       </c>
       <c r="I55" t="str">
         <f>LOOKUP(A55,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J55" t="str">
         <f>LOOKUP(B55,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3443,11 +3413,11 @@
       </c>
       <c r="L55" t="str">
         <f>LOOKUP(D55,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M55" t="str">
         <f>LOOKUP(E55,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N55" t="str">
         <f>LOOKUP(F55,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3456,7 +3426,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
         <v>13</v>
@@ -3465,10 +3435,10 @@
         <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F56" t="s">
         <v>55</v>
@@ -3478,11 +3448,11 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E21-F1-I0-</v>
+        <v>A30-C0-D0-L30-E21-F1-I0-</v>
       </c>
       <c r="I56" t="str">
         <f>LOOKUP(A56,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J56" t="str">
         <f>LOOKUP(B56,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3494,11 +3464,11 @@
       </c>
       <c r="L56" t="str">
         <f>LOOKUP(D56,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M56" t="str">
         <f>LOOKUP(E56,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N56" t="str">
         <f>LOOKUP(F56,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3507,7 +3477,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
         <v>13</v>
@@ -3516,10 +3486,10 @@
         <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="F57" t="s">
         <v>55</v>
@@ -3529,11 +3499,11 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E22-F1-I0-</v>
+        <v>A30-C0-D0-L30-E22-F1-I0-</v>
       </c>
       <c r="I57" t="str">
         <f>LOOKUP(A57,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J57" t="str">
         <f>LOOKUP(B57,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3545,11 +3515,11 @@
       </c>
       <c r="L57" t="str">
         <f>LOOKUP(D57,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M57" t="str">
         <f>LOOKUP(E57,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N57" t="str">
         <f>LOOKUP(F57,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3558,7 +3528,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -3567,10 +3537,10 @@
         <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F58" t="s">
         <v>55</v>
@@ -3580,11 +3550,11 @@
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E23-F1-I0-</v>
+        <v>A30-C0-D0-L30-E23-F1-I0-</v>
       </c>
       <c r="I58" t="str">
         <f>LOOKUP(A58,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J58" t="str">
         <f>LOOKUP(B58,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3596,11 +3566,11 @@
       </c>
       <c r="L58" t="str">
         <f>LOOKUP(D58,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M58" t="str">
         <f>LOOKUP(E58,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N58" t="str">
         <f>LOOKUP(F58,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3609,7 +3579,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
         <v>13</v>
@@ -3618,10 +3588,10 @@
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F59" t="s">
         <v>55</v>
@@ -3631,11 +3601,11 @@
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E24-F1-I0-</v>
+        <v>A30-C0-D0-L30-E24-F1-I0-</v>
       </c>
       <c r="I59" t="str">
         <f>LOOKUP(A59,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J59" t="str">
         <f>LOOKUP(B59,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3647,11 +3617,11 @@
       </c>
       <c r="L59" t="str">
         <f>LOOKUP(D59,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M59" t="str">
         <f>LOOKUP(E59,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N59" t="str">
         <f>LOOKUP(F59,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3660,7 +3630,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B60" t="s">
         <v>13</v>
@@ -3669,10 +3639,10 @@
         <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F60" t="s">
         <v>55</v>
@@ -3682,11 +3652,11 @@
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E25-F1-I0-</v>
+        <v>A30-C0-D0-L30-E25-F1-I0-</v>
       </c>
       <c r="I60" t="str">
         <f>LOOKUP(A60,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J60" t="str">
         <f>LOOKUP(B60,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3698,11 +3668,11 @@
       </c>
       <c r="L60" t="str">
         <f>LOOKUP(D60,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M60" t="str">
         <f>LOOKUP(E60,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N60" t="str">
         <f>LOOKUP(F60,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3711,7 +3681,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
         <v>13</v>
@@ -3720,10 +3690,10 @@
         <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F61" t="s">
         <v>55</v>
@@ -3733,11 +3703,11 @@
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E26-F1-I0-</v>
+        <v>A30-C0-D0-L30-E26-F1-I0-</v>
       </c>
       <c r="I61" t="str">
         <f>LOOKUP(A61,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J61" t="str">
         <f>LOOKUP(B61,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3749,11 +3719,11 @@
       </c>
       <c r="L61" t="str">
         <f>LOOKUP(D61,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M61" t="str">
         <f>LOOKUP(E61,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N61" t="str">
         <f>LOOKUP(F61,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3762,7 +3732,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
         <v>13</v>
@@ -3771,10 +3741,10 @@
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F62" t="s">
         <v>55</v>
@@ -3784,11 +3754,11 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E27-F1-I0-</v>
+        <v>A30-C0-D0-L30-E27-F1-I0-</v>
       </c>
       <c r="I62" t="str">
         <f>LOOKUP(A62,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J62" t="str">
         <f>LOOKUP(B62,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3800,11 +3770,11 @@
       </c>
       <c r="L62" t="str">
         <f>LOOKUP(D62,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M62" t="str">
         <f>LOOKUP(E62,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N62" t="str">
         <f>LOOKUP(F62,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3813,7 +3783,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
         <v>13</v>
@@ -3822,10 +3792,10 @@
         <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F63" t="s">
         <v>55</v>
@@ -3835,11 +3805,11 @@
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E28-F1-I0-</v>
+        <v>A30-C0-D0-L30-E28-F1-I0-</v>
       </c>
       <c r="I63" t="str">
         <f>LOOKUP(A63,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J63" t="str">
         <f>LOOKUP(B63,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3851,11 +3821,11 @@
       </c>
       <c r="L63" t="str">
         <f>LOOKUP(D63,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M63" t="str">
         <f>LOOKUP(E63,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N63" t="str">
         <f>LOOKUP(F63,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3864,7 +3834,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
@@ -3873,10 +3843,10 @@
         <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F64" t="s">
         <v>55</v>
@@ -3886,11 +3856,11 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>A10-C0-D0-L10-E29-F1-I0-</v>
+        <v>A30-C0-D0-L30-E29-F1-I0-</v>
       </c>
       <c r="I64" t="str">
         <f>LOOKUP(A64,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish age</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="J64" t="str">
         <f>LOOKUP(B64,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3902,11 +3872,11 @@
       </c>
       <c r="L64" t="str">
         <f>LOOKUP(D64,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>fish length</v>
+        <v>fish &amp; surv length</v>
       </c>
       <c r="M64" t="str">
         <f>LOOKUP(E64,descriptions!$C:$C,descriptions!$D:$D)</f>
-        <v>M150</v>
+        <v>internal</v>
       </c>
       <c r="N64" t="str">
         <f>LOOKUP(F64,descriptions!$C:$C,descriptions!$D:$D)</f>
@@ -3927,7 +3897,7 @@
         <v>17</v>
       </c>
       <c r="E65" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F65" t="s">
         <v>55</v>
@@ -4155,10 +4125,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,7 +4173,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C31" si="0">CONCATENATE(A3,B3)</f>
+        <f t="shared" ref="C3:C41" si="0">CONCATENATE(A3,B3)</f>
         <v>A10</v>
       </c>
       <c r="D3" t="s">
@@ -4402,7 +4372,7 @@
         <v>E10</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4417,7 +4387,7 @@
         <v>E11</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4432,7 +4402,7 @@
         <v>E12</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -4447,7 +4417,7 @@
         <v>E13</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -4462,7 +4432,7 @@
         <v>E14</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4477,7 +4447,7 @@
         <v>E15</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -4492,7 +4462,7 @@
         <v>E16</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -4507,7 +4477,7 @@
         <v>E17</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -4522,7 +4492,7 @@
         <v>E18</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -4537,96 +4507,246 @@
         <v>E19</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>F0</v>
+        <v>E20</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
-        <v>F1</v>
+        <v>E21</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>E22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>23</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>E23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30">
+        <v>24</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>E24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>E25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>E26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>27</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>E27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>28</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>E28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
+        <v>29</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>E29</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>57</v>
       </c>
-      <c r="B28">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>F0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>F1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38">
         <v>2</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C38" t="str">
         <f t="shared" si="0"/>
         <v>F2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
+      <c r="B39">
         <v>10</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C39" t="str">
         <f t="shared" si="0"/>
         <v>L10</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D39" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>44</v>
       </c>
-      <c r="B30">
+      <c r="B40">
         <v>30</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C40" t="str">
         <f t="shared" si="0"/>
         <v>L30</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>44</v>
       </c>
-      <c r="B31">
+      <c r="B41">
         <v>31</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C41" t="str">
         <f t="shared" si="0"/>
         <v>L31</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D41" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>